<commit_message>
Think i fixed memb-issues
</commit_message>
<xml_diff>
--- a/SporsmålNidarus.xlsx
+++ b/SporsmålNidarus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Documents/NTNU/Prosjekt-S22/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Documents/NTNU/Prosjekt-S22/drikkelek2022-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468E2076-3293-8141-8804-35D37DDD7493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041F5187-092A-D84F-BEA3-0DAC546D169E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="153">
   <si>
     <t>Kategori</t>
   </si>
@@ -178,9 +178,6 @@
     <t>Den som bryter må chugge drikken sin</t>
   </si>
   <si>
-    <t>Ok, red flagg eller dealbreaker:</t>
-  </si>
-  <si>
     <t>Personen studerer på Dragvoll</t>
   </si>
   <si>
@@ -229,21 +226,6 @@
     <t>Hvem ville gitt den beste lap dancen?</t>
   </si>
   <si>
-    <t>Regel</t>
-  </si>
-  <si>
-    <t>Ikke lov til å drikke med høyre hånd</t>
-  </si>
-  <si>
-    <t>Hvis regelen brytes må man ta en straffeslurk</t>
-  </si>
-  <si>
-    <t>Ikke lov til å bruke fornavn</t>
-  </si>
-  <si>
-    <t>Ikke lov til å peke ved hjelp av armene</t>
-  </si>
-  <si>
     <t>Drikk antall pek</t>
   </si>
   <si>
@@ -281,9 +263,6 @@
   </si>
   <si>
     <t>Drikk hvis du er nyshava</t>
-  </si>
-  <si>
-    <t>Jeg har aldri røyket noe sterkere enn hasj</t>
   </si>
   <si>
     <t>Hvem er mest fornøyd med eget utseende?</t>
@@ -349,31 +328,19 @@
     <t>memb: fortell om ditt siste ligg, og ranger opplevelsen fra 1-10</t>
   </si>
   <si>
-    <t>memb, legg ut på instastory: "Det er på samfundet det skjer i kveld!" eller chugg hele drikken din</t>
-  </si>
-  <si>
     <t>memb: legg ut en selfie på instastory, eller chugg hele drikken din</t>
   </si>
   <si>
     <t>memb, legg ut en boomerang på instastory, eller chiúgg hele drikken din</t>
   </si>
   <si>
-    <t>memb, legg ut på mystory: "Noen som vet hvor folk drar ut i kveld?" eller chugg hele drikken din</t>
-  </si>
-  <si>
     <t xml:space="preserve">memb må sitte på fanget til memb2 de neste 3 spørsmålene, eller chugge drikken sin. </t>
-  </si>
-  <si>
-    <t>memb: hold en tale og takk alle for å ha kommet i kveld, eller chugg hele drikken din.</t>
   </si>
   <si>
     <t>memb: gi et kompliment til hver person i rommet. Skål for komplimentene!</t>
   </si>
   <si>
     <t xml:space="preserve">memb: beskriv hver person i rommet med ett ord, og del ut 5 slurker. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karaoke!! Memb må synge et vers av sin yndlingssang, eller chugge hele drikken sin. </t>
   </si>
   <si>
     <t xml:space="preserve">memb, hvem i rommet har den beste drikken? Bytt drikke med denne personen. </t>
@@ -386,12 +353,6 @@
   </si>
   <si>
     <t>Drikk hvis du mener du er blant de 5 mest attraktive i rommet</t>
-  </si>
-  <si>
-    <t>Memb, gi 2 slurker til den som lukter best</t>
-  </si>
-  <si>
-    <t>Memb, gi to slurker til den som snakker mest</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -417,12 +378,129 @@
   <si>
     <t>memb, gå inn på insta og lik et gammelt bilde hos den første personen som dukker opp på feeden din. Eller ta 5 slurker.</t>
   </si>
+  <si>
+    <t>Ok, red flag eller dealbreaker:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Personen liker trøndersk kebab</t>
+  </si>
+  <si>
+    <t>Chuggekonkurranse!!</t>
+  </si>
+  <si>
+    <t>memb mot memb2</t>
+  </si>
+  <si>
+    <t>memb mot memb3</t>
+  </si>
+  <si>
+    <t>memb mot memb4</t>
+  </si>
+  <si>
+    <t>memb mot memb5</t>
+  </si>
+  <si>
+    <t>Hvem har finest outfit?</t>
+  </si>
+  <si>
+    <t>Hvem har finest øyne?</t>
+  </si>
+  <si>
+    <t>Hvem hadde vært den beste ektefellen?</t>
+  </si>
+  <si>
+    <t>Hvem kommer ikke inn på utested i kveld?</t>
+  </si>
+  <si>
+    <t>memb, del ut 4 slurker til den keegeste i rommet</t>
+  </si>
+  <si>
+    <t>Personen går med siving-ringen til vanlig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb: hold en tale og takk alle for å ha kommet i kveld. Del ut 5 slurker. </t>
+  </si>
+  <si>
+    <t>Jeg har aldri blitt drita på bedpress</t>
+  </si>
+  <si>
+    <t>Jeg har aldri gått meg vill på stripa</t>
+  </si>
+  <si>
+    <t>Drikk hvis du har vært keen på en fadder</t>
+  </si>
+  <si>
+    <t>Drikk hvis du har vært på et midtsidebilde</t>
+  </si>
+  <si>
+    <t>Jeg har aldri spandert drikke på en random på byen</t>
+  </si>
+  <si>
+    <t>Drikk hvis du har vært drita på festningen</t>
+  </si>
+  <si>
+    <t>memb, hva er din beste pulesang? Spill av sangen!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, hvem ville du laget frokost til? Personen får tre slurker. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, hvem ville du invitert på overnatting? Personen får 2 slurker. </t>
+  </si>
+  <si>
+    <t>Hvem har best musikksmak? Personen kan queue tre sanger.</t>
+  </si>
+  <si>
+    <t>Drikk hvis du flyttet til trondheim i år</t>
+  </si>
+  <si>
+    <t>Hvem koker mest?</t>
+  </si>
+  <si>
+    <t>memb og memb2 skal ta håndbak</t>
+  </si>
+  <si>
+    <t>memb, beskriv ditt beste ligg med tre ord. Ta en skål for hvert ord.</t>
+  </si>
+  <si>
+    <t>memb: la alle på vorset signere armen din, eller chugg drikken din</t>
+  </si>
+  <si>
+    <t>memb, lag en drink til memb2 av ting du finner på vorset</t>
+  </si>
+  <si>
+    <t>memb, hva er oddsen for at du lar memb2 klippe håret ditt?</t>
+  </si>
+  <si>
+    <t>Jeg har aldri tatt noe sterkere enn hasj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karaoke!! memb må synge et vers av sin yndlingssang, eller chugge hele drikken sin. </t>
+  </si>
+  <si>
+    <t>memb, gi 2 slurker til den som lukter best</t>
+  </si>
+  <si>
+    <t>memb, gi to slurker til den som snakker mest</t>
+  </si>
+  <si>
+    <t>memb, finn frem et glass, og la alle helle litt av drikken sin i det. Chugg glasset!</t>
+  </si>
+  <si>
+    <t>memb, drikk 3 slurker</t>
+  </si>
+  <si>
+    <t>memb, legg ut på instastory: \"Det er på samfundet det skjer i kveld!\" eller chugg hele drikken din</t>
+  </si>
+  <si>
+    <t>memb, legg ut på mystory: \"Noen som vet hvor folk drar ut i kveld?\" eller chugg hele drikken din</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -448,6 +526,12 @@
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -792,13 +876,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266B615A-CB75-A44D-9106-24B2B9F7FAAE}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="4" max="4" width="100.83203125" customWidth="1"/>
     <col min="5" max="5" width="67.6640625" customWidth="1"/>
@@ -844,7 +928,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -880,7 +964,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -916,7 +1000,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B4" s="2">
         <v>5</v>
@@ -925,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1"/>
@@ -1069,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="1"/>
@@ -1213,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="1"/>
@@ -1969,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="1"/>
@@ -2005,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="1"/>
@@ -2115,7 +2199,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="1"/>
@@ -2394,7 +2478,7 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B45" s="2">
         <v>3</v>
@@ -2403,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="1"/>
@@ -2430,7 +2514,7 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B46" s="2">
         <v>3</v>
@@ -2439,7 +2523,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="1"/>
@@ -2466,7 +2550,7 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B47" s="2">
         <v>4</v>
@@ -2475,7 +2559,7 @@
         <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="1"/>
@@ -2502,7 +2586,7 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B48" s="2">
         <v>4</v>
@@ -2511,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="1"/>
@@ -2538,7 +2622,7 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B49" s="2">
         <v>5</v>
@@ -2547,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="1"/>
@@ -2574,7 +2658,7 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B50" s="2">
         <v>7</v>
@@ -2583,7 +2667,7 @@
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="1"/>
@@ -2610,7 +2694,7 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B51" s="2">
         <v>5</v>
@@ -2619,7 +2703,7 @@
         <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="1"/>
@@ -2646,7 +2730,7 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B52" s="2">
         <v>6</v>
@@ -2655,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="1"/>
@@ -2682,7 +2766,7 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B53" s="2">
         <v>6</v>
@@ -2691,7 +2775,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="1"/>
@@ -2718,7 +2802,7 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B54" s="2">
         <v>6</v>
@@ -2727,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="1"/>
@@ -2763,7 +2847,7 @@
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="1"/>
@@ -2799,7 +2883,7 @@
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="1"/>
@@ -2835,7 +2919,7 @@
         <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="1"/>
@@ -2871,7 +2955,7 @@
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="1"/>
@@ -2907,7 +2991,7 @@
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="1"/>
@@ -2943,7 +3027,7 @@
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>46</v>
@@ -2981,7 +3065,7 @@
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="1"/>
@@ -3017,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="1"/>
@@ -3053,7 +3137,7 @@
         <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="1"/>
@@ -3089,7 +3173,7 @@
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="1"/>
@@ -3125,7 +3209,7 @@
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="1"/>
@@ -3161,7 +3245,7 @@
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="1"/>
@@ -3197,7 +3281,7 @@
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="1"/>
@@ -3233,7 +3317,7 @@
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="1"/>
@@ -3269,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="1"/>
@@ -3305,7 +3389,7 @@
         <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="1"/>
@@ -3341,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="1"/>
@@ -3368,7 +3452,7 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B72" s="2">
         <v>1</v>
@@ -3377,7 +3461,7 @@
         <v>1</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="1"/>
@@ -3404,7 +3488,7 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B73" s="2">
         <v>1</v>
@@ -3413,7 +3497,7 @@
         <v>1</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="1"/>
@@ -3440,7 +3524,7 @@
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B74" s="2">
         <v>1</v>
@@ -3449,7 +3533,7 @@
         <v>1</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="1"/>
@@ -3476,7 +3560,7 @@
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B75" s="2">
         <v>1</v>
@@ -3485,7 +3569,7 @@
         <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="1"/>
@@ -3512,7 +3596,7 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B76" s="2">
         <v>2</v>
@@ -3521,7 +3605,7 @@
         <v>1</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="1"/>
@@ -3548,7 +3632,7 @@
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="B77" s="2">
         <v>2</v>
@@ -3557,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" s="1"/>
@@ -3584,7 +3668,7 @@
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B78" s="2">
         <v>1</v>
@@ -3593,10 +3677,10 @@
         <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -3622,7 +3706,7 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B79" s="2">
         <v>1</v>
@@ -3631,10 +3715,10 @@
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -3660,7 +3744,7 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B80" s="2">
         <v>1</v>
@@ -3669,10 +3753,10 @@
         <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -3698,7 +3782,7 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B81" s="2">
         <v>1</v>
@@ -3707,10 +3791,10 @@
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -3736,7 +3820,7 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B82" s="2">
         <v>2</v>
@@ -3745,10 +3829,10 @@
         <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -3774,7 +3858,7 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B83" s="2">
         <v>3</v>
@@ -3783,10 +3867,10 @@
         <v>0</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
@@ -3812,7 +3896,7 @@
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B84" s="2">
         <v>3</v>
@@ -3821,10 +3905,10 @@
         <v>0</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -3850,7 +3934,7 @@
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B85" s="2">
         <v>4</v>
@@ -3859,10 +3943,10 @@
         <v>0</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -3888,7 +3972,7 @@
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B86" s="2">
         <v>4</v>
@@ -3897,10 +3981,10 @@
         <v>1</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
@@ -3926,7 +4010,7 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B87" s="2">
         <v>5</v>
@@ -3935,10 +4019,10 @@
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
@@ -3964,7 +4048,7 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B88" s="2">
         <v>5</v>
@@ -3973,10 +4057,10 @@
         <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -4002,7 +4086,7 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B89" s="2">
         <v>9</v>
@@ -4011,10 +4095,10 @@
         <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
@@ -4040,7 +4124,7 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="B90" s="2">
         <v>1</v>
@@ -4049,11 +4133,9 @@
         <v>0</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="E90" s="2"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
@@ -4078,7 +4160,7 @@
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="B91" s="2">
         <v>1</v>
@@ -4087,11 +4169,9 @@
         <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="E91" s="2"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -4116,7 +4196,7 @@
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="B92" s="2">
         <v>1</v>
@@ -4125,11 +4205,9 @@
         <v>0</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E92" s="2"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
@@ -4154,7 +4232,7 @@
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B93" s="2">
         <v>1</v>
@@ -4163,7 +4241,7 @@
         <v>0</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="1"/>
@@ -4190,7 +4268,7 @@
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B94" s="2">
         <v>1</v>
@@ -4199,7 +4277,7 @@
         <v>0</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="1"/>
@@ -4226,7 +4304,7 @@
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B95" s="2">
         <v>1</v>
@@ -4235,7 +4313,7 @@
         <v>0</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="1"/>
@@ -4262,7 +4340,7 @@
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B96" s="2">
         <v>1</v>
@@ -4271,7 +4349,7 @@
         <v>0</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="1"/>
@@ -4298,7 +4376,7 @@
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B97" s="2">
         <v>1</v>
@@ -4307,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="1"/>
@@ -4334,7 +4412,7 @@
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B98" s="2">
         <v>1</v>
@@ -4343,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="1"/>
@@ -4370,7 +4448,7 @@
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B99" s="2">
         <v>1</v>
@@ -4379,7 +4457,7 @@
         <v>0</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="1"/>
@@ -4406,16 +4484,16 @@
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="B100" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C100" s="2">
         <v>0</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="1"/>
@@ -4442,7 +4520,7 @@
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="B101" s="2">
         <v>1</v>
@@ -4451,7 +4529,7 @@
         <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="1"/>
@@ -4478,7 +4556,7 @@
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="B102" s="2">
         <v>1</v>
@@ -4487,7 +4565,7 @@
         <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="1"/>
@@ -4517,13 +4595,13 @@
         <v>45</v>
       </c>
       <c r="B103" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C103" s="2">
         <v>0</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="1"/>
@@ -4553,13 +4631,13 @@
         <v>45</v>
       </c>
       <c r="B104" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C104" s="2">
         <v>0</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>111</v>
+        <v>146</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="1"/>
@@ -4589,13 +4667,13 @@
         <v>45</v>
       </c>
       <c r="B105" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C105" s="2">
         <v>0</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="1"/>
@@ -4625,13 +4703,13 @@
         <v>45</v>
       </c>
       <c r="B106" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C106" s="2">
         <v>0</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="1"/>
@@ -4661,13 +4739,13 @@
         <v>45</v>
       </c>
       <c r="B107" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C107" s="2">
         <v>0</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107" s="1"/>
@@ -4703,7 +4781,7 @@
         <v>0</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="E108" s="2"/>
       <c r="F108" s="1"/>
@@ -4733,13 +4811,13 @@
         <v>45</v>
       </c>
       <c r="B109" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C109" s="2">
         <v>0</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109" s="1"/>
@@ -4769,15 +4847,15 @@
         <v>45</v>
       </c>
       <c r="B110" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C110" s="2">
         <v>0</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E110" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
@@ -4805,15 +4883,15 @@
         <v>45</v>
       </c>
       <c r="B111" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C111" s="2">
         <v>0</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E111" s="2"/>
+        <v>147</v>
+      </c>
+      <c r="E111" s="1"/>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
@@ -4836,20 +4914,20 @@
       <c r="Y111" s="1"/>
       <c r="Z111" s="1"/>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B112" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C112" s="2">
         <v>0</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E112" s="2"/>
+      <c r="D112" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
@@ -4874,16 +4952,13 @@
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B113" s="2">
-        <v>4</v>
+        <v>114</v>
       </c>
       <c r="C113" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -4909,16 +4984,16 @@
       <c r="Z113" s="1"/>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B114" s="2">
+      <c r="A114" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B114" s="1">
         <v>1</v>
       </c>
-      <c r="C114" s="2">
+      <c r="C114" s="1">
         <v>0</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D114" s="1" t="s">
         <v>117</v>
       </c>
       <c r="E114" s="1"/>
@@ -4944,17 +5019,17 @@
       <c r="Y114" s="1"/>
       <c r="Z114" s="1"/>
     </row>
-    <row r="115" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A115" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B115" s="2">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B115" s="1">
         <v>1</v>
       </c>
-      <c r="C115" s="2">
+      <c r="C115" s="1">
         <v>0</v>
       </c>
-      <c r="D115" s="4" t="s">
+      <c r="D115" s="1" t="s">
         <v>118</v>
       </c>
       <c r="E115" s="1"/>
@@ -4981,6 +5056,18 @@
       <c r="Z115" s="1"/>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" s="1">
+        <v>1</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
@@ -5005,10 +5092,18 @@
       <c r="Z116" s="1"/>
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
+      <c r="A117" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117" s="1">
+        <v>1</v>
+      </c>
+      <c r="C117" s="1">
+        <v>0</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
@@ -5033,10 +5128,18 @@
       <c r="Z117" s="1"/>
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
+      <c r="A118" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B118" s="1">
+        <v>6</v>
+      </c>
+      <c r="C118" s="1">
+        <v>0</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
@@ -5061,10 +5164,18 @@
       <c r="Z118" s="1"/>
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
+      <c r="A119" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B119" s="1">
+        <v>1</v>
+      </c>
+      <c r="C119" s="1">
+        <v>0</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>121</v>
+      </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
@@ -5089,10 +5200,18 @@
       <c r="Z119" s="1"/>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
-      <c r="D120" s="1"/>
+      <c r="A120" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B120" s="1">
+        <v>1</v>
+      </c>
+      <c r="C120" s="1">
+        <v>0</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
@@ -5117,10 +5236,18 @@
       <c r="Z120" s="1"/>
     </row>
     <row r="121" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="1"/>
+      <c r="A121" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B121" s="1">
+        <v>1</v>
+      </c>
+      <c r="C121" s="1">
+        <v>0</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
@@ -5145,10 +5272,18 @@
       <c r="Z121" s="1"/>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
+      <c r="A122" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B122" s="1">
+        <v>1</v>
+      </c>
+      <c r="C122" s="1">
+        <v>0</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
@@ -5173,10 +5308,18 @@
       <c r="Z122" s="1"/>
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
+      <c r="A123" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B123" s="1">
+        <v>1</v>
+      </c>
+      <c r="C123" s="1">
+        <v>0</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
@@ -5201,10 +5344,18 @@
       <c r="Z123" s="1"/>
     </row>
     <row r="124" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="C124" s="1"/>
-      <c r="D124" s="1"/>
+      <c r="A124" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B124" s="1">
+        <v>1</v>
+      </c>
+      <c r="C124" s="1">
+        <v>0</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
@@ -5229,10 +5380,18 @@
       <c r="Z124" s="1"/>
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="1"/>
+      <c r="A125" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B125" s="1">
+        <v>1</v>
+      </c>
+      <c r="C125" s="1">
+        <v>1</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
@@ -5257,10 +5416,18 @@
       <c r="Z125" s="1"/>
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
-      <c r="C126" s="1"/>
-      <c r="D126" s="1"/>
+      <c r="A126" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B126" s="1">
+        <v>2</v>
+      </c>
+      <c r="C126" s="1">
+        <v>1</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
@@ -5285,10 +5452,18 @@
       <c r="Z126" s="1"/>
     </row>
     <row r="127" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
-      <c r="C127" s="1"/>
-      <c r="D127" s="1"/>
+      <c r="A127" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B127" s="1">
+        <v>1</v>
+      </c>
+      <c r="C127" s="1">
+        <v>1</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
@@ -5313,10 +5488,18 @@
       <c r="Z127" s="1"/>
     </row>
     <row r="128" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
-      <c r="C128" s="1"/>
-      <c r="D128" s="1"/>
+      <c r="A128" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B128" s="1">
+        <v>1</v>
+      </c>
+      <c r="C128" s="1">
+        <v>1</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
@@ -5341,10 +5524,18 @@
       <c r="Z128" s="1"/>
     </row>
     <row r="129" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A129" s="1"/>
-      <c r="B129" s="1"/>
-      <c r="C129" s="1"/>
-      <c r="D129" s="1"/>
+      <c r="A129" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129" s="1">
+        <v>1</v>
+      </c>
+      <c r="C129" s="1">
+        <v>1</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
@@ -5369,10 +5560,18 @@
       <c r="Z129" s="1"/>
     </row>
     <row r="130" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
-      <c r="D130" s="1"/>
+      <c r="A130" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B130" s="1">
+        <v>1</v>
+      </c>
+      <c r="C130" s="1">
+        <v>1</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
@@ -5397,10 +5596,18 @@
       <c r="Z130" s="1"/>
     </row>
     <row r="131" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A131" s="1"/>
-      <c r="B131" s="1"/>
-      <c r="C131" s="1"/>
-      <c r="D131" s="1"/>
+      <c r="A131" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131" s="1">
+        <v>1</v>
+      </c>
+      <c r="C131" s="1">
+        <v>1</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
@@ -5425,10 +5632,18 @@
       <c r="Z131" s="1"/>
     </row>
     <row r="132" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
-      <c r="C132" s="1"/>
-      <c r="D132" s="1"/>
+      <c r="A132" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B132" s="1">
+        <v>4</v>
+      </c>
+      <c r="C132" s="1">
+        <v>0</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
@@ -5453,10 +5668,18 @@
       <c r="Z132" s="1"/>
     </row>
     <row r="133" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A133" s="1"/>
-      <c r="B133" s="1"/>
-      <c r="C133" s="1"/>
-      <c r="D133" s="1"/>
+      <c r="A133" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B133" s="1">
+        <v>5</v>
+      </c>
+      <c r="C133" s="1">
+        <v>0</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
@@ -5481,10 +5704,18 @@
       <c r="Z133" s="1"/>
     </row>
     <row r="134" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A134" s="1"/>
-      <c r="B134" s="1"/>
-      <c r="C134" s="1"/>
-      <c r="D134" s="1"/>
+      <c r="A134" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B134" s="1">
+        <v>5</v>
+      </c>
+      <c r="C134" s="1">
+        <v>0</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
@@ -5509,10 +5740,18 @@
       <c r="Z134" s="1"/>
     </row>
     <row r="135" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A135" s="1"/>
-      <c r="B135" s="1"/>
-      <c r="C135" s="1"/>
-      <c r="D135" s="1"/>
+      <c r="A135" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B135" s="1">
+        <v>1</v>
+      </c>
+      <c r="C135" s="1">
+        <v>0</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
@@ -5537,10 +5776,18 @@
       <c r="Z135" s="1"/>
     </row>
     <row r="136" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A136" s="1"/>
-      <c r="B136" s="1"/>
-      <c r="C136" s="1"/>
-      <c r="D136" s="1"/>
+      <c r="A136" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B136" s="1">
+        <v>1</v>
+      </c>
+      <c r="C136" s="1">
+        <v>1</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
@@ -5565,10 +5812,18 @@
       <c r="Z136" s="1"/>
     </row>
     <row r="137" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A137" s="1"/>
-      <c r="B137" s="1"/>
-      <c r="C137" s="1"/>
-      <c r="D137" s="1"/>
+      <c r="A137" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B137" s="1">
+        <v>1</v>
+      </c>
+      <c r="C137" s="1">
+        <v>1</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
@@ -5593,10 +5848,18 @@
       <c r="Z137" s="1"/>
     </row>
     <row r="138" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A138" s="1"/>
-      <c r="B138" s="1"/>
-      <c r="C138" s="1"/>
-      <c r="D138" s="1"/>
+      <c r="A138" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B138" s="1">
+        <v>1</v>
+      </c>
+      <c r="C138" s="1">
+        <v>0</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
@@ -5621,10 +5884,18 @@
       <c r="Z138" s="1"/>
     </row>
     <row r="139" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A139" s="1"/>
-      <c r="B139" s="1"/>
-      <c r="C139" s="1"/>
-      <c r="D139" s="1"/>
+      <c r="A139" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B139" s="1">
+        <v>6</v>
+      </c>
+      <c r="C139" s="1">
+        <v>0</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
@@ -5649,10 +5920,16 @@
       <c r="Z139" s="1"/>
     </row>
     <row r="140" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A140" s="1"/>
-      <c r="B140" s="1"/>
+      <c r="A140" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B140" s="1">
+        <v>3</v>
+      </c>
       <c r="C140" s="1"/>
-      <c r="D140" s="1"/>
+      <c r="D140" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
@@ -5677,10 +5954,16 @@
       <c r="Z140" s="1"/>
     </row>
     <row r="141" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A141" s="1"/>
-      <c r="B141" s="1"/>
+      <c r="A141" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B141" s="1">
+        <v>2</v>
+      </c>
       <c r="C141" s="1"/>
-      <c r="D141" s="1"/>
+      <c r="D141" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
@@ -5705,10 +5988,18 @@
       <c r="Z141" s="1"/>
     </row>
     <row r="142" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A142" s="1"/>
-      <c r="B142" s="1"/>
-      <c r="C142" s="1"/>
-      <c r="D142" s="1"/>
+      <c r="A142" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B142" s="1">
+        <v>10</v>
+      </c>
+      <c r="C142" s="1">
+        <v>0</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
@@ -5733,10 +6024,18 @@
       <c r="Z142" s="1"/>
     </row>
     <row r="143" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A143" s="1"/>
-      <c r="B143" s="1"/>
-      <c r="C143" s="1"/>
-      <c r="D143" s="1"/>
+      <c r="A143" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B143" s="1">
+        <v>2</v>
+      </c>
+      <c r="C143" s="1">
+        <v>0</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
@@ -5760,12 +6059,19 @@
       <c r="Y143" s="1"/>
       <c r="Z143" s="1"/>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
-      <c r="C144" s="1"/>
-      <c r="D144" s="1"/>
-      <c r="E144" s="1"/>
+    <row r="144" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B144" s="1">
+        <v>2</v>
+      </c>
+      <c r="C144" s="1">
+        <v>0</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
@@ -5788,12 +6094,19 @@
       <c r="Y144" s="1"/>
       <c r="Z144" s="1"/>
     </row>
-    <row r="145" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A145" s="1"/>
-      <c r="B145" s="1"/>
-      <c r="C145" s="1"/>
-      <c r="D145" s="1"/>
-      <c r="E145" s="1"/>
+    <row r="145" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B145" s="1">
+        <v>2</v>
+      </c>
+      <c r="C145" s="1">
+        <v>0</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
@@ -5817,11 +6130,6 @@
       <c r="Z145" s="1"/>
     </row>
     <row r="146" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A146" s="1"/>
-      <c r="B146" s="1"/>
-      <c r="C146" s="1"/>
-      <c r="D146" s="1"/>
-      <c r="E146" s="1"/>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
@@ -29761,6 +30069,7 @@
     <sortCondition ref="A2:A259"/>
     <sortCondition ref="B2:B259"/>
   </sortState>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed memb-issue, updated addQuestions-modal
</commit_message>
<xml_diff>
--- a/SporsmålNidarus.xlsx
+++ b/SporsmålNidarus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Documents/NTNU/Prosjekt-S22/drikkelek2022-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C454DA-CC31-E04A-95DC-EA33E17A73F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC351A2-82DA-4F4D-B007-912FFDEE1D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="148">
   <si>
     <t>Kategori</t>
   </si>
@@ -383,15 +383,6 @@
   </si>
   <si>
     <t>memb mot memb2</t>
-  </si>
-  <si>
-    <t>memb mot memb3</t>
-  </si>
-  <si>
-    <t>memb mot memb4</t>
-  </si>
-  <si>
-    <t>memb mot memb5</t>
   </si>
   <si>
     <t>Hvem har finest outfit?</t>
@@ -870,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266B615A-CB75-A44D-9106-24B2B9F7FAAE}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2589,7 +2580,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="1"/>
@@ -4523,7 +4514,7 @@
         <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="1"/>
@@ -4559,7 +4550,7 @@
         <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="1"/>
@@ -4595,7 +4586,7 @@
         <v>0</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="1"/>
@@ -4703,7 +4694,7 @@
         <v>0</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="1"/>
@@ -4811,7 +4802,7 @@
         <v>0</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -4847,7 +4838,7 @@
         <v>0</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
@@ -4952,7 +4943,7 @@
         <v>0</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -4988,7 +4979,7 @@
         <v>0</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
@@ -5024,7 +5015,7 @@
         <v>0</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -5060,7 +5051,7 @@
         <v>0</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -5096,7 +5087,7 @@
         <v>0</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -5132,7 +5123,7 @@
         <v>0</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -5168,7 +5159,7 @@
         <v>0</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -5204,7 +5195,7 @@
         <v>0</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
@@ -5276,7 +5267,7 @@
         <v>0</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
@@ -5312,7 +5303,7 @@
         <v>1</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
@@ -5348,7 +5339,7 @@
         <v>1</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
@@ -5384,7 +5375,7 @@
         <v>1</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -5420,7 +5411,7 @@
         <v>1</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -5456,7 +5447,7 @@
         <v>1</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -5492,7 +5483,7 @@
         <v>1</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
@@ -5528,7 +5519,7 @@
         <v>1</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -5564,7 +5555,7 @@
         <v>0</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -5600,7 +5591,7 @@
         <v>0</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
@@ -5636,7 +5627,7 @@
         <v>0</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
@@ -5672,7 +5663,7 @@
         <v>0</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
@@ -5708,7 +5699,7 @@
         <v>1</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
@@ -5744,7 +5735,7 @@
         <v>1</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
@@ -5780,7 +5771,7 @@
         <v>0</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
@@ -5816,7 +5807,7 @@
         <v>0</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -5850,7 +5841,7 @@
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -5884,7 +5875,7 @@
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -5920,7 +5911,7 @@
         <v>0</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
@@ -5956,7 +5947,7 @@
         <v>0</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
@@ -5992,7 +5983,7 @@
         <v>0</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
@@ -6027,7 +6018,7 @@
         <v>0</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>

</xml_diff>

<commit_message>
fixed difficulty-scale, and cleaned up Questions-compnent
</commit_message>
<xml_diff>
--- a/SporsmålNidarus.xlsx
+++ b/SporsmålNidarus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Documents/NTNU/Prosjekt-S22/drikkelek2022-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC351A2-82DA-4F4D-B007-912FFDEE1D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1EA774-D7F7-1C4C-BFE7-142A36642EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="145">
   <si>
     <t>Kategori</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Drikk hvis du har pult noen i rommet</t>
-  </si>
-  <si>
-    <t>Drikk hvis du skal pule en i rommet</t>
   </si>
   <si>
     <t>Drikk hvis du har pult de siste 24 timene</t>
@@ -202,9 +199,6 @@
     <t>Hvem har finest smil?</t>
   </si>
   <si>
-    <t>Hvem har den sjukeste historien?</t>
-  </si>
-  <si>
     <t>Hvem er kåtest?</t>
   </si>
   <si>
@@ -215,9 +209,6 @@
   </si>
   <si>
     <t>Hvem har tatt flest angrepiller?</t>
-  </si>
-  <si>
-    <t>Hvem ville gitt den beste lap dancen?</t>
   </si>
   <si>
     <t>Drikk antall pek</t>
@@ -295,9 +286,6 @@
     <t>memb skal ta av seg buksene, og kan ta dem på etter minst 3 runder. </t>
   </si>
   <si>
-    <t>memb må hooke noen i rommet</t>
-  </si>
-  <si>
     <t>memb og memb2 må bytte drikke </t>
   </si>
   <si>
@@ -323,9 +311,6 @@
   </si>
   <si>
     <t>memb: legg ut en selfie på instastory, eller chugg hele drikken din</t>
-  </si>
-  <si>
-    <t>memb, legg ut en boomerang på instastory, eller chiúgg hele drikken din</t>
   </si>
   <si>
     <t xml:space="preserve">memb må sitte på fanget til memb2 de neste 3 spørsmålene, eller chugge drikken sin. </t>
@@ -364,9 +349,6 @@
     <t>memb kan legge til en utfordring</t>
   </si>
   <si>
-    <t>legge til utfordring</t>
-  </si>
-  <si>
     <t>memb må ta av tre klesplagg, og ha dem av de neste 3 rundene</t>
   </si>
   <si>
@@ -377,12 +359,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Personen liker trøndersk kebab</t>
-  </si>
-  <si>
-    <t>Chuggekonkurranse!!</t>
-  </si>
-  <si>
-    <t>memb mot memb2</t>
   </si>
   <si>
     <t>Hvem har finest outfit?</t>
@@ -401,9 +377,6 @@
   </si>
   <si>
     <t>Personen går med siving-ringen til vanlig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">memb: hold en tale og takk alle for å ha kommet i kveld. Del ut 5 slurker. </t>
   </si>
   <si>
     <t>Jeg har aldri blitt drita på bedpress</t>
@@ -479,6 +452,24 @@
   </si>
   <si>
     <t>memb, legg ut på mystory: \"Noen som vet hvor folk drar ut i kveld?\" eller chugg hele drikken din</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hvem har den sjukeste historien? Fortell historien. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hvem ville gitt den beste lap dancen? Gi en lap dance til en valgfri person. </t>
+  </si>
+  <si>
+    <t>Drikk hvis du skal pule noen i rommet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb må hooke noen i rommet, eller ta 5 slurker. </t>
+  </si>
+  <si>
+    <t>Chuggekonkurranse! memb mot memb2</t>
+  </si>
+  <si>
+    <t>legg til utfordring</t>
   </si>
 </sst>
 </file>
@@ -859,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266B615A-CB75-A44D-9106-24B2B9F7FAAE}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -913,7 +904,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B2" s="2">
         <v>5</v>
@@ -922,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="1"/>
@@ -1066,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1"/>
@@ -1210,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1"/>
@@ -1282,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="1"/>
@@ -1318,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="1"/>
@@ -1354,7 +1345,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="1"/>
@@ -1390,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="1"/>
@@ -1426,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="1"/>
@@ -1462,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="1"/>
@@ -1489,7 +1480,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
@@ -1498,7 +1489,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="1"/>
@@ -1525,7 +1516,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2">
         <v>1</v>
@@ -1534,7 +1525,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="1"/>
@@ -1561,7 +1552,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>1</v>
@@ -1570,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="1"/>
@@ -1597,7 +1588,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2">
         <v>2</v>
@@ -1606,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="1"/>
@@ -1633,7 +1624,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="2">
         <v>2</v>
@@ -1642,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="1"/>
@@ -1669,7 +1660,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="2">
         <v>2</v>
@@ -1678,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="1"/>
@@ -1705,7 +1696,7 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="2">
         <v>2</v>
@@ -1714,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="1"/>
@@ -1741,7 +1732,7 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="2">
         <v>2</v>
@@ -1750,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="1"/>
@@ -1777,7 +1768,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="2">
         <v>2</v>
@@ -1786,7 +1777,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="1"/>
@@ -1813,7 +1804,7 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="2">
         <v>3</v>
@@ -1822,7 +1813,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="1"/>
@@ -1849,7 +1840,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" s="2">
         <v>3</v>
@@ -1858,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="1"/>
@@ -1885,7 +1876,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="2">
         <v>3</v>
@@ -1894,7 +1885,7 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="1"/>
@@ -1921,7 +1912,7 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" s="2">
         <v>3</v>
@@ -1930,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="1"/>
@@ -1957,7 +1948,7 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="2">
         <v>3</v>
@@ -1966,7 +1957,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="1"/>
@@ -1993,7 +1984,7 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" s="2">
         <v>3</v>
@@ -2002,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="1"/>
@@ -2029,7 +2020,7 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="2">
         <v>4</v>
@@ -2038,10 +2029,10 @@
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2067,7 +2058,7 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="2">
         <v>4</v>
@@ -2076,7 +2067,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="1"/>
@@ -2103,7 +2094,7 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" s="2">
         <v>4</v>
@@ -2112,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="1"/>
@@ -2139,7 +2130,7 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" s="2">
         <v>4</v>
@@ -2148,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="1"/>
@@ -2175,7 +2166,7 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" s="2">
         <v>4</v>
@@ -2184,7 +2175,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="1"/>
@@ -2211,7 +2202,7 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" s="2">
         <v>4</v>
@@ -2220,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="1"/>
@@ -2247,7 +2238,7 @@
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" s="2">
         <v>4</v>
@@ -2256,7 +2247,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="1"/>
@@ -2283,7 +2274,7 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" s="2">
         <v>4</v>
@@ -2292,7 +2283,7 @@
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="1"/>
@@ -2319,7 +2310,7 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" s="2">
         <v>4</v>
@@ -2328,7 +2319,7 @@
         <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="1"/>
@@ -2355,7 +2346,7 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42" s="2">
         <v>4</v>
@@ -2364,7 +2355,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="1"/>
@@ -2391,7 +2382,7 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B43" s="2">
         <v>3</v>
@@ -2400,7 +2391,7 @@
         <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="1"/>
@@ -2427,7 +2418,7 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B44" s="2">
         <v>3</v>
@@ -2436,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="1"/>
@@ -2463,7 +2454,7 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B45" s="2">
         <v>4</v>
@@ -2472,7 +2463,7 @@
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="1"/>
@@ -2499,7 +2490,7 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B46" s="2">
         <v>4</v>
@@ -2508,7 +2499,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="1"/>
@@ -2535,7 +2526,7 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B47" s="2">
         <v>5</v>
@@ -2544,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="1"/>
@@ -2571,7 +2562,7 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B48" s="2">
         <v>7</v>
@@ -2580,7 +2571,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="1"/>
@@ -2607,7 +2598,7 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B49" s="2">
         <v>5</v>
@@ -2616,7 +2607,7 @@
         <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="1"/>
@@ -2643,7 +2634,7 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B50" s="2">
         <v>6</v>
@@ -2652,7 +2643,7 @@
         <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="1"/>
@@ -2679,7 +2670,7 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B51" s="2">
         <v>6</v>
@@ -2688,7 +2679,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="1"/>
@@ -2715,7 +2706,7 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B52" s="2">
         <v>6</v>
@@ -2724,7 +2715,7 @@
         <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="1"/>
@@ -2751,7 +2742,7 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B53" s="2">
         <v>1</v>
@@ -2760,7 +2751,7 @@
         <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="1"/>
@@ -2787,7 +2778,7 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B54" s="2">
         <v>1</v>
@@ -2796,7 +2787,7 @@
         <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="1"/>
@@ -2823,7 +2814,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B55" s="2">
         <v>1</v>
@@ -2832,7 +2823,7 @@
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="1"/>
@@ -2859,7 +2850,7 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B56" s="2">
         <v>1</v>
@@ -2868,7 +2859,7 @@
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="1"/>
@@ -2895,7 +2886,7 @@
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B57" s="2">
         <v>1</v>
@@ -2904,7 +2895,7 @@
         <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="1"/>
@@ -2931,7 +2922,7 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B58" s="2">
         <v>2</v>
@@ -2940,10 +2931,10 @@
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -2969,7 +2960,7 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B59" s="2">
         <v>4</v>
@@ -2978,7 +2969,7 @@
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="1"/>
@@ -3005,7 +2996,7 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B60" s="2">
         <v>4</v>
@@ -3014,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="1"/>
@@ -3041,7 +3032,7 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B61" s="2">
         <v>4</v>
@@ -3050,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="1"/>
@@ -3077,7 +3068,7 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B62" s="2">
         <v>4</v>
@@ -3086,7 +3077,7 @@
         <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="1"/>
@@ -3113,7 +3104,7 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B63" s="2">
         <v>4</v>
@@ -3122,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="1"/>
@@ -3149,7 +3140,7 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B64" s="2">
         <v>5</v>
@@ -3158,7 +3149,7 @@
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="1"/>
@@ -3185,7 +3176,7 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B65" s="2">
         <v>6</v>
@@ -3194,7 +3185,7 @@
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="1"/>
@@ -3221,7 +3212,7 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B66" s="2">
         <v>9</v>
@@ -3230,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="1"/>
@@ -3257,7 +3248,7 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B67" s="2">
         <v>9</v>
@@ -3266,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="1"/>
@@ -3293,7 +3284,7 @@
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B68" s="2">
         <v>9</v>
@@ -3302,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="1"/>
@@ -3329,7 +3320,7 @@
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B69" s="2">
         <v>10</v>
@@ -3338,7 +3329,7 @@
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="1"/>
@@ -3365,7 +3356,7 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B70" s="2">
         <v>1</v>
@@ -3374,7 +3365,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="1"/>
@@ -3401,7 +3392,7 @@
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B71" s="2">
         <v>1</v>
@@ -3410,7 +3401,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="1"/>
@@ -3437,7 +3428,7 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B72" s="2">
         <v>1</v>
@@ -3446,7 +3437,7 @@
         <v>1</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="1"/>
@@ -3473,7 +3464,7 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B73" s="2">
         <v>1</v>
@@ -3482,7 +3473,7 @@
         <v>1</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="1"/>
@@ -3509,7 +3500,7 @@
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B74" s="2">
         <v>2</v>
@@ -3518,7 +3509,7 @@
         <v>1</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="1"/>
@@ -3545,7 +3536,7 @@
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B75" s="2">
         <v>2</v>
@@ -3554,7 +3545,7 @@
         <v>1</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="1"/>
@@ -3581,7 +3572,7 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B76" s="2">
         <v>1</v>
@@ -3590,10 +3581,10 @@
         <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -3619,7 +3610,7 @@
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B77" s="2">
         <v>1</v>
@@ -3628,10 +3619,10 @@
         <v>0</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -3657,7 +3648,7 @@
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B78" s="2">
         <v>1</v>
@@ -3666,10 +3657,10 @@
         <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -3695,7 +3686,7 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B79" s="2">
         <v>1</v>
@@ -3704,10 +3695,10 @@
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
@@ -3733,7 +3724,7 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B80" s="2">
         <v>2</v>
@@ -3742,10 +3733,10 @@
         <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
@@ -3771,7 +3762,7 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B81" s="2">
         <v>3</v>
@@ -3780,10 +3771,10 @@
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
@@ -3809,7 +3800,7 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B82" s="2">
         <v>3</v>
@@ -3818,10 +3809,10 @@
         <v>0</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
@@ -3847,7 +3838,7 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B83" s="2">
         <v>4</v>
@@ -3856,10 +3847,10 @@
         <v>0</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
@@ -3885,7 +3876,7 @@
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B84" s="2">
         <v>4</v>
@@ -3894,10 +3885,10 @@
         <v>1</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
@@ -3923,7 +3914,7 @@
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B85" s="2">
         <v>5</v>
@@ -3932,10 +3923,10 @@
         <v>0</v>
       </c>
       <c r="D85" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
@@ -3961,7 +3952,7 @@
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B86" s="2">
         <v>5</v>
@@ -3970,10 +3961,10 @@
         <v>0</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
@@ -3999,7 +3990,7 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B87" s="2">
         <v>9</v>
@@ -4008,10 +3999,10 @@
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
@@ -4037,7 +4028,7 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B88" s="2">
         <v>1</v>
@@ -4046,7 +4037,7 @@
         <v>0</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="1"/>
@@ -4073,7 +4064,7 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B89" s="2">
         <v>1</v>
@@ -4082,7 +4073,7 @@
         <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" s="1"/>
@@ -4109,7 +4100,7 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B90" s="2">
         <v>1</v>
@@ -4118,7 +4109,7 @@
         <v>0</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="1"/>
@@ -4145,7 +4136,7 @@
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B91" s="2">
         <v>1</v>
@@ -4154,7 +4145,7 @@
         <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="1"/>
@@ -4181,7 +4172,7 @@
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B92" s="2">
         <v>1</v>
@@ -4190,7 +4181,7 @@
         <v>0</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="1"/>
@@ -4217,7 +4208,7 @@
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B93" s="2">
         <v>1</v>
@@ -4226,7 +4217,7 @@
         <v>0</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="1"/>
@@ -4253,7 +4244,7 @@
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B94" s="2">
         <v>1</v>
@@ -4262,7 +4253,7 @@
         <v>0</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="1"/>
@@ -4289,7 +4280,7 @@
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B95" s="2">
         <v>1</v>
@@ -4298,7 +4289,7 @@
         <v>0</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="1"/>
@@ -4325,7 +4316,7 @@
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B96" s="2">
         <v>1</v>
@@ -4334,7 +4325,7 @@
         <v>0</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E96" s="2"/>
       <c r="F96" s="1"/>
@@ -4361,7 +4352,7 @@
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>109</v>
+        <v>144</v>
       </c>
       <c r="B97" s="2">
         <v>1</v>
@@ -4370,7 +4361,7 @@
         <v>0</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="1"/>
@@ -4397,7 +4388,7 @@
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B98" s="2">
         <v>6</v>
@@ -4406,7 +4397,7 @@
         <v>0</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="1"/>
@@ -4433,7 +4424,7 @@
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B99" s="2">
         <v>1</v>
@@ -4442,7 +4433,7 @@
         <v>0</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="1"/>
@@ -4469,7 +4460,7 @@
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B100" s="2">
         <v>1</v>
@@ -4478,7 +4469,7 @@
         <v>0</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="1"/>
@@ -4505,16 +4496,16 @@
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B101" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C101" s="2">
         <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="1"/>
@@ -4541,16 +4532,16 @@
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B102" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C102" s="2">
         <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="1"/>
@@ -4577,16 +4568,16 @@
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B103" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C103" s="2">
         <v>0</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="1"/>
@@ -4613,16 +4604,16 @@
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B104" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C104" s="2">
         <v>0</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="1"/>
@@ -4649,7 +4640,7 @@
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B105" s="2">
         <v>5</v>
@@ -4658,7 +4649,7 @@
         <v>0</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="1"/>
@@ -4685,18 +4676,18 @@
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B106" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C106" s="2">
         <v>0</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E106" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="E106" s="1"/>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
@@ -4721,18 +4712,18 @@
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B107" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C107" s="2">
         <v>0</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E107" s="2"/>
+        <v>133</v>
+      </c>
+      <c r="E107" s="1"/>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
@@ -4755,18 +4746,18 @@
       <c r="Y107" s="1"/>
       <c r="Z107" s="1"/>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B108" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C108" s="2">
         <v>0</v>
       </c>
-      <c r="D108" s="2" t="s">
-        <v>111</v>
+      <c r="D108" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
@@ -4793,16 +4784,13 @@
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B109" s="2">
+        <v>106</v>
+      </c>
+      <c r="C109" s="2">
         <v>1</v>
       </c>
-      <c r="C109" s="2">
-        <v>0</v>
-      </c>
       <c r="D109" s="2" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -4827,17 +4815,17 @@
       <c r="Y109" s="1"/>
       <c r="Z109" s="1"/>
     </row>
-    <row r="110" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B110" s="2">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B110" s="1">
         <v>1</v>
       </c>
-      <c r="C110" s="2">
+      <c r="C110" s="1">
         <v>0</v>
       </c>
-      <c r="D110" s="4" t="s">
+      <c r="D110" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E110" s="1"/>
@@ -4864,14 +4852,17 @@
       <c r="Z110" s="1"/>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A111" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C111" s="2">
+      <c r="A111" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B111" s="1">
         <v>1</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>113</v>
+      <c r="C111" s="1">
+        <v>0</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
@@ -4898,7 +4889,7 @@
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>114</v>
+        <v>42</v>
       </c>
       <c r="B112" s="1">
         <v>1</v>
@@ -4907,7 +4898,7 @@
         <v>0</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
@@ -4934,7 +4925,7 @@
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>114</v>
+        <v>42</v>
       </c>
       <c r="B113" s="1">
         <v>1</v>
@@ -4943,7 +4934,7 @@
         <v>0</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
@@ -4970,16 +4961,16 @@
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>114</v>
+        <v>42</v>
       </c>
       <c r="B114" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C114" s="1">
         <v>0</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
@@ -5006,7 +4997,7 @@
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="B115" s="1">
         <v>1</v>
@@ -5015,7 +5006,7 @@
         <v>0</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -5042,16 +5033,16 @@
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B116" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C116" s="1">
         <v>0</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -5078,7 +5069,7 @@
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B117" s="1">
         <v>1</v>
@@ -5087,7 +5078,7 @@
         <v>0</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -5114,7 +5105,7 @@
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B118" s="1">
         <v>1</v>
@@ -5123,7 +5114,7 @@
         <v>0</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -5150,7 +5141,7 @@
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B119" s="1">
         <v>1</v>
@@ -5158,8 +5149,8 @@
       <c r="C119" s="1">
         <v>0</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>118</v>
+      <c r="D119" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -5186,7 +5177,7 @@
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B120" s="1">
         <v>1</v>
@@ -5195,7 +5186,7 @@
         <v>0</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
@@ -5221,17 +5212,17 @@
       <c r="Z120" s="1"/>
     </row>
     <row r="121" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A121" s="1" t="s">
-        <v>43</v>
+      <c r="A121" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="B121" s="1">
         <v>1</v>
       </c>
       <c r="C121" s="1">
-        <v>0</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>77</v>
+        <v>1</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
@@ -5258,16 +5249,16 @@
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B122" s="1">
+        <v>2</v>
+      </c>
+      <c r="C122" s="1">
         <v>1</v>
       </c>
-      <c r="C122" s="1">
-        <v>0</v>
-      </c>
       <c r="D122" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
@@ -5293,8 +5284,8 @@
       <c r="Z122" s="1"/>
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A123" s="2" t="s">
-        <v>112</v>
+      <c r="A123" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B123" s="1">
         <v>1</v>
@@ -5303,7 +5294,7 @@
         <v>1</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
@@ -5330,16 +5321,16 @@
     </row>
     <row r="124" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B124" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C124" s="1">
         <v>1</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
@@ -5366,7 +5357,7 @@
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B125" s="1">
         <v>1</v>
@@ -5375,7 +5366,7 @@
         <v>1</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -5402,7 +5393,7 @@
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B126" s="1">
         <v>1</v>
@@ -5411,7 +5402,7 @@
         <v>1</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -5441,13 +5432,13 @@
         <v>5</v>
       </c>
       <c r="B127" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C127" s="1">
         <v>1</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -5474,16 +5465,16 @@
     </row>
     <row r="128" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B128" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C128" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
@@ -5510,16 +5501,16 @@
     </row>
     <row r="129" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B129" s="1">
         <v>5</v>
       </c>
-      <c r="B129" s="1">
-        <v>1</v>
-      </c>
       <c r="C129" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -5546,16 +5537,16 @@
     </row>
     <row r="130" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B130" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C130" s="1">
         <v>0</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -5582,16 +5573,16 @@
     </row>
     <row r="131" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B131" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C131" s="1">
         <v>0</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
@@ -5618,16 +5609,16 @@
     </row>
     <row r="132" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B132" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C132" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
@@ -5654,16 +5645,16 @@
     </row>
     <row r="133" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B133" s="1">
         <v>1</v>
       </c>
       <c r="C133" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
@@ -5690,16 +5681,16 @@
     </row>
     <row r="134" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B134" s="1">
         <v>1</v>
       </c>
       <c r="C134" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
@@ -5726,16 +5717,16 @@
     </row>
     <row r="135" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B135" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C135" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
@@ -5762,16 +5753,16 @@
     </row>
     <row r="136" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B136" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C136" s="1">
         <v>0</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
@@ -5798,16 +5789,16 @@
     </row>
     <row r="137" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B137" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C137" s="1">
         <v>0</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
@@ -5834,14 +5825,16 @@
     </row>
     <row r="138" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B138" s="1">
-        <v>3</v>
-      </c>
-      <c r="C138" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="C138" s="1">
+        <v>0</v>
+      </c>
       <c r="D138" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -5868,14 +5861,16 @@
     </row>
     <row r="139" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B139" s="1">
         <v>2</v>
       </c>
-      <c r="C139" s="1"/>
+      <c r="C139" s="1">
+        <v>0</v>
+      </c>
       <c r="D139" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -5900,20 +5895,19 @@
       <c r="Y139" s="1"/>
       <c r="Z139" s="1"/>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B140" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C140" s="1">
         <v>0</v>
       </c>
-      <c r="D140" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E140" s="1"/>
+      <c r="D140" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
@@ -5936,9 +5930,9 @@
       <c r="Y140" s="1"/>
       <c r="Z140" s="1"/>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B141" s="1">
         <v>2</v>
@@ -5946,10 +5940,9 @@
       <c r="C141" s="1">
         <v>0</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E141" s="1"/>
+      <c r="D141" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
@@ -5972,19 +5965,7 @@
       <c r="Y141" s="1"/>
       <c r="Z141" s="1"/>
     </row>
-    <row r="142" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A142" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B142" s="1">
-        <v>2</v>
-      </c>
-      <c r="C142" s="1">
-        <v>0</v>
-      </c>
-      <c r="D142" s="4" t="s">
-        <v>145</v>
-      </c>
+    <row r="142" spans="1:26" x14ac:dyDescent="0.2">
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
@@ -6007,19 +5988,12 @@
       <c r="Y142" s="1"/>
       <c r="Z142" s="1"/>
     </row>
-    <row r="143" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B143" s="1">
-        <v>2</v>
-      </c>
-      <c r="C143" s="1">
-        <v>0</v>
-      </c>
-      <c r="D143" s="4" t="s">
-        <v>145</v>
-      </c>
+    <row r="143" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="1"/>
+      <c r="D143" s="1"/>
+      <c r="E143" s="1"/>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
@@ -6043,6 +6017,11 @@
       <c r="Z143" s="1"/>
     </row>
     <row r="144" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+      <c r="C144" s="1"/>
+      <c r="D144" s="1"/>
+      <c r="E144" s="1"/>
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
@@ -11106,11 +11085,6 @@
       <c r="Z324" s="1"/>
     </row>
     <row r="325" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A325" s="1"/>
-      <c r="B325" s="1"/>
-      <c r="C325" s="1"/>
-      <c r="D325" s="1"/>
-      <c r="E325" s="1"/>
       <c r="F325" s="1"/>
       <c r="G325" s="1"/>
       <c r="H325" s="1"/>
@@ -11134,11 +11108,6 @@
       <c r="Z325" s="1"/>
     </row>
     <row r="326" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A326" s="1"/>
-      <c r="B326" s="1"/>
-      <c r="C326" s="1"/>
-      <c r="D326" s="1"/>
-      <c r="E326" s="1"/>
       <c r="F326" s="1"/>
       <c r="G326" s="1"/>
       <c r="H326" s="1"/>
@@ -11162,6 +11131,11 @@
       <c r="Z326" s="1"/>
     </row>
     <row r="327" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A327" s="1"/>
+      <c r="B327" s="1"/>
+      <c r="C327" s="1"/>
+      <c r="D327" s="1"/>
+      <c r="E327" s="1"/>
       <c r="F327" s="1"/>
       <c r="G327" s="1"/>
       <c r="H327" s="1"/>
@@ -11185,6 +11159,11 @@
       <c r="Z327" s="1"/>
     </row>
     <row r="328" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A328" s="1"/>
+      <c r="B328" s="1"/>
+      <c r="C328" s="1"/>
+      <c r="D328" s="1"/>
+      <c r="E328" s="1"/>
       <c r="F328" s="1"/>
       <c r="G328" s="1"/>
       <c r="H328" s="1"/>
@@ -29967,66 +29946,10 @@
       <c r="Y998" s="1"/>
       <c r="Z998" s="1"/>
     </row>
-    <row r="999" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A999" s="1"/>
-      <c r="B999" s="1"/>
-      <c r="C999" s="1"/>
-      <c r="D999" s="1"/>
-      <c r="E999" s="1"/>
-      <c r="F999" s="1"/>
-      <c r="G999" s="1"/>
-      <c r="H999" s="1"/>
-      <c r="I999" s="1"/>
-      <c r="J999" s="1"/>
-      <c r="K999" s="1"/>
-      <c r="L999" s="1"/>
-      <c r="M999" s="1"/>
-      <c r="N999" s="1"/>
-      <c r="O999" s="1"/>
-      <c r="P999" s="1"/>
-      <c r="Q999" s="1"/>
-      <c r="R999" s="1"/>
-      <c r="S999" s="1"/>
-      <c r="T999" s="1"/>
-      <c r="U999" s="1"/>
-      <c r="V999" s="1"/>
-      <c r="W999" s="1"/>
-      <c r="X999" s="1"/>
-      <c r="Y999" s="1"/>
-      <c r="Z999" s="1"/>
-    </row>
-    <row r="1000" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1000" s="1"/>
-      <c r="B1000" s="1"/>
-      <c r="C1000" s="1"/>
-      <c r="D1000" s="1"/>
-      <c r="E1000" s="1"/>
-      <c r="F1000" s="1"/>
-      <c r="G1000" s="1"/>
-      <c r="H1000" s="1"/>
-      <c r="I1000" s="1"/>
-      <c r="J1000" s="1"/>
-      <c r="K1000" s="1"/>
-      <c r="L1000" s="1"/>
-      <c r="M1000" s="1"/>
-      <c r="N1000" s="1"/>
-      <c r="O1000" s="1"/>
-      <c r="P1000" s="1"/>
-      <c r="Q1000" s="1"/>
-      <c r="R1000" s="1"/>
-      <c r="S1000" s="1"/>
-      <c r="T1000" s="1"/>
-      <c r="U1000" s="1"/>
-      <c r="V1000" s="1"/>
-      <c r="W1000" s="1"/>
-      <c r="X1000" s="1"/>
-      <c r="Y1000" s="1"/>
-      <c r="Z1000" s="1"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E259">
-    <sortCondition ref="A2:A259"/>
-    <sortCondition ref="B2:B259"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E257">
+    <sortCondition ref="A2:A257"/>
+    <sortCondition ref="B2:B257"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added and implementet glos-theme-button
</commit_message>
<xml_diff>
--- a/SporsmålNidarus.xlsx
+++ b/SporsmålNidarus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Documents/NTNU/Prosjekt-S22/drikkelek2022-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1EA774-D7F7-1C4C-BFE7-142A36642EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A91420-6D8E-A142-A734-16F3E6A852A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="158">
   <si>
     <t>Kategori</t>
   </si>
@@ -271,9 +271,6 @@
     <t>memb  kan dele ut 4 slurker til den som lukter best</t>
   </si>
   <si>
-    <t>memb og memb2 må ha øyekontakt de neste fem spørsmålene</t>
-  </si>
-  <si>
     <t>memb må si sin største fetish, eller ta 4 slurker </t>
   </si>
   <si>
@@ -470,6 +467,48 @@
   </si>
   <si>
     <t>legg til utfordring</t>
+  </si>
+  <si>
+    <t>Drikk hvis du har væt i milla</t>
+  </si>
+  <si>
+    <t>Personen har gått på folkehøyskole</t>
+  </si>
+  <si>
+    <t>Jeg har aldri vært på cava-søndag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, alle kan stille deg et spørsmål hver. Svar ærlig, eller drikk 5 slurker. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stirrekonkurranse mellom memb1 og memb2. Vinneren deler ut 6 slurker. </t>
+  </si>
+  <si>
+    <t>memb, drikk 2 slurker</t>
+  </si>
+  <si>
+    <t>memb, drikk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, send melding til ditt siste ligg og si at du har fått klamma. Eller drikk 5 slurker. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, hvem ville du byttet liv med? Personen får 3 slurker. </t>
+  </si>
+  <si>
+    <t>Utfordring</t>
+  </si>
+  <si>
+    <t>Ta en runde med vann eller vodka</t>
+  </si>
+  <si>
+    <t>Hvem har mest kontroll på livet?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drikk hvis du søkte indøk. Chugg hvis du kom inn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drikk hvis du har kjørt elsparkesykkel på fylla. </t>
   </si>
 </sst>
 </file>
@@ -852,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266B615A-CB75-A44D-9106-24B2B9F7FAAE}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -904,16 +943,16 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2">
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="1"/>
@@ -946,10 +985,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>97</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1"/>
@@ -982,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1"/>
@@ -1021,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="1"/>
@@ -1054,10 +1093,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1"/>
@@ -1090,10 +1129,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="1"/>
@@ -1119,19 +1158,19 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
-        <v>2</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2"/>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1155,19 +1194,19 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2"/>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1191,19 +1230,19 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="2"/>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1231,15 +1270,14 @@
         <v>5</v>
       </c>
       <c r="B11" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>144</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1263,19 +1301,19 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="2">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
         <v>0</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" s="2"/>
+      <c r="D12" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1303,13 +1341,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="1"/>
@@ -1335,19 +1373,19 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="2">
-        <v>7</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="2"/>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1371,19 +1409,19 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2">
-        <v>8</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="2"/>
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1411,13 +1449,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C16" s="2">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="1"/>
@@ -1447,13 +1485,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="1"/>
@@ -1480,16 +1518,16 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="1"/>
@@ -1516,16 +1554,16 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>20</v>
+        <v>140</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="1"/>
@@ -1552,16 +1590,16 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="1"/>
@@ -1588,16 +1626,16 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="1"/>
@@ -1624,16 +1662,16 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="1"/>
@@ -1660,16 +1698,16 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="1"/>
@@ -1696,16 +1734,16 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="1"/>
@@ -1735,13 +1773,13 @@
         <v>18</v>
       </c>
       <c r="B25" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="1"/>
@@ -1771,13 +1809,13 @@
         <v>18</v>
       </c>
       <c r="B26" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="1"/>
@@ -1807,13 +1845,13 @@
         <v>18</v>
       </c>
       <c r="B27" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="1"/>
@@ -1839,19 +1877,19 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="2">
-        <v>3</v>
-      </c>
-      <c r="C28" s="2">
+      <c r="B28" s="1">
         <v>1</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="2"/>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1875,19 +1913,19 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="2">
-        <v>3</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B29" s="1">
         <v>1</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="2"/>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -1915,13 +1953,13 @@
         <v>18</v>
       </c>
       <c r="B30" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="2">
         <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="1"/>
@@ -1951,13 +1989,13 @@
         <v>18</v>
       </c>
       <c r="B31" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="2">
         <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="1"/>
@@ -1987,13 +2025,13 @@
         <v>18</v>
       </c>
       <c r="B32" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="1"/>
@@ -2023,17 +2061,15 @@
         <v>18</v>
       </c>
       <c r="B33" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E33" s="2"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2061,13 +2097,13 @@
         <v>18</v>
       </c>
       <c r="B34" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C34" s="2">
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="1"/>
@@ -2097,13 +2133,13 @@
         <v>18</v>
       </c>
       <c r="B35" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="1"/>
@@ -2129,19 +2165,19 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="2">
-        <v>4</v>
-      </c>
-      <c r="C36" s="2">
+      <c r="B36" s="1">
+        <v>2</v>
+      </c>
+      <c r="C36" s="1">
         <v>1</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="2"/>
+      <c r="D36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2165,19 +2201,19 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="2">
-        <v>4</v>
-      </c>
-      <c r="C37" s="2">
+      <c r="B37" s="1">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1">
         <v>1</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" s="2"/>
+      <c r="D37" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2205,13 +2241,13 @@
         <v>18</v>
       </c>
       <c r="B38" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="1"/>
@@ -2241,13 +2277,13 @@
         <v>18</v>
       </c>
       <c r="B39" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="1"/>
@@ -2277,13 +2313,13 @@
         <v>18</v>
       </c>
       <c r="B40" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="1"/>
@@ -2313,13 +2349,13 @@
         <v>18</v>
       </c>
       <c r="B41" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="1"/>
@@ -2349,13 +2385,13 @@
         <v>18</v>
       </c>
       <c r="B42" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="1"/>
@@ -2382,16 +2418,16 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B43" s="2">
         <v>3</v>
       </c>
       <c r="C43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="1"/>
@@ -2417,17 +2453,17 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>59</v>
+      <c r="A44" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B44" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44" s="2">
         <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="1"/>
@@ -2454,7 +2490,7 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B45" s="2">
         <v>4</v>
@@ -2463,7 +2499,7 @@
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="1"/>
@@ -2489,8 +2525,8 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>59</v>
+      <c r="A46" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B46" s="2">
         <v>4</v>
@@ -2499,7 +2535,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="1"/>
@@ -2525,19 +2561,21 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>59</v>
+      <c r="A47" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B47" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -2562,16 +2600,16 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B48" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C48" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>131</v>
+        <v>34</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="1"/>
@@ -2597,17 +2635,17 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>59</v>
+      <c r="A49" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B49" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="1"/>
@@ -2634,16 +2672,16 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B50" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C50" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="1"/>
@@ -2670,16 +2708,16 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B51" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="1"/>
@@ -2706,16 +2744,16 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="B52" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="1"/>
@@ -2742,16 +2780,16 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B53" s="2">
+        <v>4</v>
+      </c>
+      <c r="C53" s="2">
         <v>1</v>
       </c>
-      <c r="C53" s="2">
-        <v>0</v>
-      </c>
       <c r="D53" s="2" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="1"/>
@@ -2778,16 +2816,16 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B54" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C54" s="2">
         <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="1"/>
@@ -2813,17 +2851,17 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>42</v>
+      <c r="A55" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B55" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C55" s="2">
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="1"/>
@@ -2850,16 +2888,16 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B56" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C56" s="2">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="1"/>
@@ -2885,17 +2923,17 @@
       <c r="Z56" s="1"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>42</v>
+      <c r="A57" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B57" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="1"/>
@@ -2921,21 +2959,19 @@
       <c r="Z57" s="1"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>42</v>
+      <c r="A58" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B58" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C58" s="2">
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E58" s="2"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
@@ -2959,17 +2995,17 @@
       <c r="Z58" s="1"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>42</v>
+      <c r="A59" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B59" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="1"/>
@@ -2996,16 +3032,16 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C60" s="2">
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="1"/>
@@ -3032,16 +3068,16 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B61" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C61" s="2">
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="1"/>
@@ -3068,16 +3104,16 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B62" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="1"/>
@@ -3104,16 +3140,16 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B63" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C63" s="2">
         <v>0</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="1"/>
@@ -3140,16 +3176,16 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B64" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C64" s="2">
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="1"/>
@@ -3176,16 +3212,16 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B65" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C65" s="2">
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="1"/>
@@ -3212,16 +3248,16 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B66" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C66" s="2">
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="1"/>
@@ -3248,16 +3284,16 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B67" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C67" s="2">
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="1"/>
@@ -3284,16 +3320,16 @@
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B68" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C68" s="2">
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="1"/>
@@ -3320,16 +3356,16 @@
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B69" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C69" s="2">
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="1"/>
@@ -3356,16 +3392,16 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>106</v>
+        <v>143</v>
       </c>
       <c r="B70" s="2">
         <v>1</v>
       </c>
       <c r="C70" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="1"/>
@@ -3392,16 +3428,16 @@
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>106</v>
+        <v>143</v>
       </c>
       <c r="B71" s="2">
         <v>1</v>
       </c>
       <c r="C71" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="1"/>
@@ -3428,16 +3464,16 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>106</v>
+        <v>143</v>
       </c>
       <c r="B72" s="2">
         <v>1</v>
       </c>
       <c r="C72" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="1"/>
@@ -3464,16 +3500,16 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>106</v>
+        <v>143</v>
       </c>
       <c r="B73" s="2">
         <v>1</v>
       </c>
       <c r="C73" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="1"/>
@@ -3500,16 +3536,16 @@
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="B74" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="1"/>
@@ -3536,16 +3572,16 @@
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="B75" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C75" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="1"/>
@@ -3572,7 +3608,7 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B76" s="2">
         <v>1</v>
@@ -3581,11 +3617,9 @@
         <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="E76" s="2"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
@@ -3610,7 +3644,7 @@
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B77" s="2">
         <v>1</v>
@@ -3619,11 +3653,9 @@
         <v>0</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E77" s="2"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
@@ -3648,7 +3680,7 @@
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B78" s="2">
         <v>1</v>
@@ -3657,11 +3689,9 @@
         <v>0</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E78" s="2"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
@@ -3686,7 +3716,7 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B79" s="2">
         <v>1</v>
@@ -3695,11 +3725,9 @@
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="E79" s="2"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
@@ -3724,20 +3752,18 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B80" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C80" s="2">
         <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E80" s="2"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
@@ -3762,20 +3788,18 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B81" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C81" s="2">
         <v>0</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
@@ -3798,22 +3822,20 @@
       <c r="Y81" s="1"/>
       <c r="Z81" s="1"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B82" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C82" s="2">
         <v>0</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="D82" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
@@ -3837,21 +3859,19 @@
       <c r="Z82" s="1"/>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B83" s="2">
-        <v>4</v>
-      </c>
-      <c r="C83" s="2">
+      <c r="A83" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B83" s="1">
+        <v>1</v>
+      </c>
+      <c r="C83" s="1">
         <v>0</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="D83" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
@@ -3875,21 +3895,19 @@
       <c r="Z83" s="1"/>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B84" s="2">
-        <v>4</v>
-      </c>
-      <c r="C84" s="2">
+      <c r="A84" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B84" s="1">
         <v>1</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="C84" s="1">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
@@ -3913,21 +3931,19 @@
       <c r="Z84" s="1"/>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B85" s="2">
-        <v>5</v>
-      </c>
-      <c r="C85" s="2">
+      <c r="A85" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B85" s="1">
+        <v>1</v>
+      </c>
+      <c r="C85" s="1">
         <v>0</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="D85" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
@@ -3951,21 +3967,19 @@
       <c r="Z85" s="1"/>
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B86" s="2">
-        <v>5</v>
-      </c>
-      <c r="C86" s="2">
+      <c r="A86" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1">
         <v>0</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="D86" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
@@ -3989,21 +4003,19 @@
       <c r="Z86" s="1"/>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A87" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B87" s="2">
-        <v>9</v>
-      </c>
-      <c r="C87" s="2">
+      <c r="A87" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B87" s="1">
+        <v>1</v>
+      </c>
+      <c r="C87" s="1">
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>86</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
@@ -4027,19 +4039,19 @@
       <c r="Z87" s="1"/>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B88" s="2">
+      <c r="A88" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B88" s="1">
         <v>1</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88" s="1">
         <v>0</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E88" s="2"/>
+      <c r="D88" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
@@ -4063,19 +4075,19 @@
       <c r="Z88" s="1"/>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B89" s="2">
+      <c r="A89" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" s="1">
         <v>1</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="1">
         <v>0</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E89" s="2"/>
+      <c r="D89" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
@@ -4099,19 +4111,19 @@
       <c r="Z89" s="1"/>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B90" s="2">
+      <c r="A90" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B90" s="1">
         <v>1</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90" s="1">
         <v>0</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E90" s="2"/>
+      <c r="D90" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
@@ -4136,18 +4148,20 @@
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
       <c r="B91" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C91" s="2">
         <v>0</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E91" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -4171,19 +4185,19 @@
       <c r="Z91" s="1"/>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A92" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B92" s="2">
-        <v>1</v>
-      </c>
-      <c r="C92" s="2">
+      <c r="A92" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B92" s="1">
+        <v>2</v>
+      </c>
+      <c r="C92" s="1">
         <v>0</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E92" s="2"/>
+      <c r="D92" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
@@ -4207,19 +4221,19 @@
       <c r="Z92" s="1"/>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A93" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B93" s="2">
-        <v>1</v>
-      </c>
-      <c r="C93" s="2">
+      <c r="A93" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B93" s="1">
+        <v>2</v>
+      </c>
+      <c r="C93" s="1">
         <v>0</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E93" s="2"/>
+      <c r="D93" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
@@ -4242,20 +4256,19 @@
       <c r="Y93" s="1"/>
       <c r="Z93" s="1"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B94" s="2">
-        <v>1</v>
-      </c>
-      <c r="C94" s="2">
+    <row r="94" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94" s="1">
+        <v>2</v>
+      </c>
+      <c r="C94" s="1">
         <v>0</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E94" s="2"/>
+      <c r="D94" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
@@ -4278,20 +4291,19 @@
       <c r="Y94" s="1"/>
       <c r="Z94" s="1"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B95" s="2">
-        <v>1</v>
-      </c>
-      <c r="C95" s="2">
+    <row r="95" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" s="1">
+        <v>2</v>
+      </c>
+      <c r="C95" s="1">
         <v>0</v>
       </c>
-      <c r="D95" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E95" s="2"/>
+      <c r="D95" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
@@ -4315,19 +4327,19 @@
       <c r="Z95" s="1"/>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B96" s="2">
-        <v>1</v>
-      </c>
-      <c r="C96" s="2">
+      <c r="A96" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B96" s="1">
+        <v>2</v>
+      </c>
+      <c r="C96" s="1">
         <v>0</v>
       </c>
-      <c r="D96" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E96" s="2"/>
+      <c r="D96" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
@@ -4351,19 +4363,19 @@
       <c r="Z96" s="1"/>
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A97" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B97" s="2">
-        <v>1</v>
-      </c>
-      <c r="C97" s="2">
+      <c r="A97" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B97" s="1">
+        <v>2</v>
+      </c>
+      <c r="C97" s="1">
         <v>0</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E97" s="2"/>
+      <c r="D97" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
@@ -4387,19 +4399,19 @@
       <c r="Z97" s="1"/>
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B98" s="2">
-        <v>6</v>
-      </c>
-      <c r="C98" s="2">
+      <c r="B98" s="1">
+        <v>3</v>
+      </c>
+      <c r="C98" s="1">
         <v>0</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E98" s="2"/>
+      <c r="D98" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
@@ -4423,19 +4435,19 @@
       <c r="Z98" s="1"/>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B99" s="2">
-        <v>1</v>
-      </c>
-      <c r="C99" s="2">
+      <c r="B99" s="1">
+        <v>3</v>
+      </c>
+      <c r="C99" s="1">
         <v>0</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E99" s="2"/>
+      <c r="D99" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
@@ -4463,13 +4475,13 @@
         <v>42</v>
       </c>
       <c r="B100" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C100" s="2">
         <v>0</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="1"/>
@@ -4499,13 +4511,13 @@
         <v>42</v>
       </c>
       <c r="B101" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C101" s="2">
         <v>0</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>132</v>
+        <v>78</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="1"/>
@@ -4535,13 +4547,13 @@
         <v>42</v>
       </c>
       <c r="B102" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C102" s="2">
         <v>0</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="1"/>
@@ -4571,7 +4583,7 @@
         <v>42</v>
       </c>
       <c r="B103" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C103" s="2">
         <v>0</v>
@@ -4607,13 +4619,13 @@
         <v>42</v>
       </c>
       <c r="B104" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C104" s="2">
         <v>0</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="1"/>
@@ -4643,15 +4655,15 @@
         <v>42</v>
       </c>
       <c r="B105" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C105" s="2">
         <v>0</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E105" s="2"/>
+        <v>104</v>
+      </c>
+      <c r="E105" s="1"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
@@ -4675,17 +4687,17 @@
       <c r="Z105" s="1"/>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B106" s="1">
         <v>4</v>
       </c>
-      <c r="C106" s="2">
+      <c r="C106" s="1">
         <v>0</v>
       </c>
-      <c r="D106" s="2" t="s">
-        <v>105</v>
+      <c r="D106" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -4715,15 +4727,15 @@
         <v>42</v>
       </c>
       <c r="B107" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C107" s="2">
         <v>0</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E107" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="E107" s="2"/>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
@@ -4746,20 +4758,20 @@
       <c r="Y107" s="1"/>
       <c r="Z107" s="1"/>
     </row>
-    <row r="108" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B108" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C108" s="2">
         <v>0</v>
       </c>
-      <c r="D108" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E108" s="1"/>
+      <c r="D108" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E108" s="2"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
@@ -4783,14 +4795,17 @@
       <c r="Z108" s="1"/>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A109" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C109" s="2">
-        <v>1</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>107</v>
+      <c r="A109" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B109" s="1">
+        <v>5</v>
+      </c>
+      <c r="C109" s="1">
+        <v>0</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -4820,13 +4835,13 @@
         <v>42</v>
       </c>
       <c r="B110" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C110" s="1">
         <v>0</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
@@ -4852,19 +4867,19 @@
       <c r="Z110" s="1"/>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
+      <c r="A111" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B111" s="1">
-        <v>1</v>
-      </c>
-      <c r="C111" s="1">
+      <c r="B111" s="2">
+        <v>6</v>
+      </c>
+      <c r="C111" s="2">
         <v>0</v>
       </c>
-      <c r="D111" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E111" s="1"/>
+      <c r="D111" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E111" s="2"/>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
@@ -4888,19 +4903,19 @@
       <c r="Z111" s="1"/>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
+      <c r="A112" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B112" s="1">
-        <v>1</v>
-      </c>
-      <c r="C112" s="1">
+      <c r="B112" s="2">
+        <v>6</v>
+      </c>
+      <c r="C112" s="2">
         <v>0</v>
       </c>
-      <c r="D112" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E112" s="1"/>
+      <c r="D112" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E112" s="2"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
@@ -4924,19 +4939,19 @@
       <c r="Z112" s="1"/>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="2">
+        <v>6</v>
+      </c>
+      <c r="C113" s="2">
         <v>1</v>
       </c>
-      <c r="C113" s="1">
-        <v>0</v>
-      </c>
-      <c r="D113" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E113" s="1"/>
+      <c r="D113" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E113" s="2"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
@@ -4960,19 +4975,19 @@
       <c r="Z113" s="1"/>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
+      <c r="A114" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="2">
         <v>6</v>
       </c>
-      <c r="C114" s="1">
+      <c r="C114" s="2">
         <v>0</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E114" s="1"/>
+      <c r="D114" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E114" s="2"/>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
@@ -4997,16 +5012,16 @@
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B115" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C115" s="1">
         <v>0</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
@@ -5033,16 +5048,16 @@
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B116" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C116" s="1">
         <v>0</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -5068,19 +5083,19 @@
       <c r="Z116" s="1"/>
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A117" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B117" s="1">
-        <v>1</v>
-      </c>
-      <c r="C117" s="1">
+      <c r="A117" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B117" s="2">
+        <v>7</v>
+      </c>
+      <c r="C117" s="2">
         <v>0</v>
       </c>
-      <c r="D117" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E117" s="1"/>
+      <c r="D117" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E117" s="2"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
@@ -5104,19 +5119,19 @@
       <c r="Z117" s="1"/>
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B118" s="1">
-        <v>1</v>
-      </c>
-      <c r="C118" s="1">
+      <c r="A118" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B118" s="2">
+        <v>8</v>
+      </c>
+      <c r="C118" s="2">
         <v>0</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E118" s="1"/>
+      <c r="D118" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E118" s="2"/>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
@@ -5144,13 +5159,13 @@
         <v>42</v>
       </c>
       <c r="B119" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C119" s="1">
         <v>0</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>74</v>
+      <c r="D119" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
@@ -5176,19 +5191,19 @@
       <c r="Z119" s="1"/>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
+      <c r="A120" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B120" s="1">
-        <v>1</v>
-      </c>
-      <c r="C120" s="1">
+      <c r="B120" s="2">
+        <v>9</v>
+      </c>
+      <c r="C120" s="2">
         <v>0</v>
       </c>
-      <c r="D120" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E120" s="1"/>
+      <c r="D120" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E120" s="2"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
@@ -5213,18 +5228,18 @@
     </row>
     <row r="121" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B121" s="1">
-        <v>1</v>
-      </c>
-      <c r="C121" s="1">
-        <v>1</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E121" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="B121" s="2">
+        <v>9</v>
+      </c>
+      <c r="C121" s="2">
+        <v>0</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E121" s="2"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
@@ -5248,19 +5263,19 @@
       <c r="Z121" s="1"/>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B122" s="1">
-        <v>2</v>
-      </c>
-      <c r="C122" s="1">
-        <v>1</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E122" s="1"/>
+      <c r="A122" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B122" s="2">
+        <v>9</v>
+      </c>
+      <c r="C122" s="2">
+        <v>0</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E122" s="2"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
@@ -5284,19 +5299,19 @@
       <c r="Z122" s="1"/>
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B123" s="1">
-        <v>1</v>
-      </c>
-      <c r="C123" s="1">
-        <v>1</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E123" s="1"/>
+      <c r="A123" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B123" s="2">
+        <v>10</v>
+      </c>
+      <c r="C123" s="2">
+        <v>0</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E123" s="2"/>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
@@ -5321,16 +5336,16 @@
     </row>
     <row r="124" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B124" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C124" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
@@ -5356,19 +5371,19 @@
       <c r="Z124" s="1"/>
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A125" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B125" s="1">
+      <c r="A125" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B125" s="2">
         <v>1</v>
       </c>
-      <c r="C125" s="1">
+      <c r="C125" s="2">
         <v>1</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E125" s="1"/>
+      <c r="D125" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E125" s="2"/>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
@@ -5392,19 +5407,19 @@
       <c r="Z125" s="1"/>
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A126" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B126" s="1">
+      <c r="A126" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B126" s="2">
         <v>1</v>
       </c>
-      <c r="C126" s="1">
+      <c r="C126" s="2">
         <v>1</v>
       </c>
-      <c r="D126" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E126" s="1"/>
+      <c r="D126" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E126" s="2"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
@@ -5428,19 +5443,19 @@
       <c r="Z126" s="1"/>
     </row>
     <row r="127" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B127" s="1">
-        <v>2</v>
-      </c>
-      <c r="C127" s="1">
+      <c r="A127" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B127" s="2">
         <v>1</v>
       </c>
-      <c r="D127" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E127" s="1"/>
+      <c r="C127" s="2">
+        <v>1</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E127" s="2"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
@@ -5464,19 +5479,19 @@
       <c r="Z127" s="1"/>
     </row>
     <row r="128" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B128" s="1">
-        <v>4</v>
-      </c>
-      <c r="C128" s="1">
-        <v>0</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E128" s="1"/>
+      <c r="A128" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B128" s="2">
+        <v>1</v>
+      </c>
+      <c r="C128" s="2">
+        <v>1</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E128" s="2"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
@@ -5500,17 +5515,17 @@
       <c r="Z128" s="1"/>
     </row>
     <row r="129" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A129" s="1" t="s">
-        <v>42</v>
+      <c r="A129" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B129" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C129" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -5536,17 +5551,17 @@
       <c r="Z129" s="1"/>
     </row>
     <row r="130" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A130" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B130" s="1">
-        <v>5</v>
-      </c>
-      <c r="C130" s="1">
-        <v>0</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>122</v>
+      <c r="A130" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B130" s="2">
+        <v>1</v>
+      </c>
+      <c r="C130" s="2">
+        <v>1</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -5572,19 +5587,18 @@
       <c r="Z130" s="1"/>
     </row>
     <row r="131" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A131" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B131" s="1">
+      <c r="A131" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B131" s="2">
         <v>1</v>
       </c>
-      <c r="C131" s="1">
+      <c r="C131" s="2">
         <v>0</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E131" s="1"/>
+      <c r="D131" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
@@ -5608,19 +5622,19 @@
       <c r="Z131" s="1"/>
     </row>
     <row r="132" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B132" s="1">
+      <c r="A132" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B132" s="2">
+        <v>2</v>
+      </c>
+      <c r="C132" s="2">
         <v>1</v>
       </c>
-      <c r="C132" s="1">
-        <v>1</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E132" s="1"/>
+      <c r="D132" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E132" s="2"/>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
@@ -5644,19 +5658,19 @@
       <c r="Z132" s="1"/>
     </row>
     <row r="133" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A133" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B133" s="1">
+      <c r="A133" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B133" s="2">
+        <v>2</v>
+      </c>
+      <c r="C133" s="2">
         <v>1</v>
       </c>
-      <c r="C133" s="1">
-        <v>1</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E133" s="1"/>
+      <c r="D133" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E133" s="2"/>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
@@ -5680,19 +5694,21 @@
       <c r="Z133" s="1"/>
     </row>
     <row r="134" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B134" s="1">
+      <c r="A134" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B134" s="2">
         <v>1</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134" s="2">
         <v>0</v>
       </c>
-      <c r="D134" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E134" s="1"/>
+      <c r="D134" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
@@ -5716,19 +5732,21 @@
       <c r="Z134" s="1"/>
     </row>
     <row r="135" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A135" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B135" s="1">
-        <v>6</v>
-      </c>
-      <c r="C135" s="1">
+      <c r="A135" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B135" s="2">
+        <v>1</v>
+      </c>
+      <c r="C135" s="2">
         <v>0</v>
       </c>
-      <c r="D135" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E135" s="1"/>
+      <c r="D135" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
@@ -5752,19 +5770,21 @@
       <c r="Z135" s="1"/>
     </row>
     <row r="136" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A136" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B136" s="1">
-        <v>3</v>
-      </c>
-      <c r="C136" s="1">
+      <c r="A136" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B136" s="2">
+        <v>1</v>
+      </c>
+      <c r="C136" s="2">
         <v>0</v>
       </c>
-      <c r="D136" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E136" s="1"/>
+      <c r="D136" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
@@ -5788,19 +5808,21 @@
       <c r="Z136" s="1"/>
     </row>
     <row r="137" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B137" s="1">
-        <v>2</v>
-      </c>
-      <c r="C137" s="1">
+      <c r="A137" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B137" s="2">
+        <v>1</v>
+      </c>
+      <c r="C137" s="2">
         <v>0</v>
       </c>
-      <c r="D137" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E137" s="1"/>
+      <c r="D137" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
@@ -5825,16 +5847,16 @@
     </row>
     <row r="138" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B138" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C138" s="1">
         <v>0</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
@@ -5861,16 +5883,16 @@
     </row>
     <row r="139" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B139" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C139" s="1">
         <v>0</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -5895,19 +5917,20 @@
       <c r="Y139" s="1"/>
       <c r="Z139" s="1"/>
     </row>
-    <row r="140" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B140" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C140" s="1">
         <v>0</v>
       </c>
-      <c r="D140" s="4" t="s">
-        <v>136</v>
-      </c>
+      <c r="D140" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E140" s="1"/>
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
@@ -5930,19 +5953,20 @@
       <c r="Y140" s="1"/>
       <c r="Z140" s="1"/>
     </row>
-    <row r="141" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B141" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C141" s="1">
         <v>0</v>
       </c>
-      <c r="D141" s="4" t="s">
-        <v>136</v>
-      </c>
+      <c r="D141" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E141" s="1"/>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
@@ -5966,6 +5990,19 @@
       <c r="Z141" s="1"/>
     </row>
     <row r="142" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B142" s="1">
+        <v>1</v>
+      </c>
+      <c r="C142" s="1">
+        <v>0</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E142" s="1"/>
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
@@ -5989,10 +6026,18 @@
       <c r="Z142" s="1"/>
     </row>
     <row r="143" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A143" s="1"/>
-      <c r="B143" s="1"/>
-      <c r="C143" s="1"/>
-      <c r="D143" s="1"/>
+      <c r="A143" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B143" s="1">
+        <v>1</v>
+      </c>
+      <c r="C143" s="1">
+        <v>1</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>124</v>
+      </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
@@ -6017,10 +6062,18 @@
       <c r="Z143" s="1"/>
     </row>
     <row r="144" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A144" s="1"/>
-      <c r="B144" s="1"/>
-      <c r="C144" s="1"/>
-      <c r="D144" s="1"/>
+      <c r="A144" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B144" s="1">
+        <v>1</v>
+      </c>
+      <c r="C144" s="1">
+        <v>0</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
@@ -6045,11 +6098,21 @@
       <c r="Z144" s="1"/>
     </row>
     <row r="145" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A145" s="1"/>
-      <c r="B145" s="1"/>
-      <c r="C145" s="1"/>
-      <c r="D145" s="1"/>
-      <c r="E145" s="1"/>
+      <c r="A145" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B145" s="2">
+        <v>2</v>
+      </c>
+      <c r="C145" s="2">
+        <v>0</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
@@ -6073,11 +6136,21 @@
       <c r="Z145" s="1"/>
     </row>
     <row r="146" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A146" s="1"/>
-      <c r="B146" s="1"/>
-      <c r="C146" s="1"/>
-      <c r="D146" s="1"/>
-      <c r="E146" s="1"/>
+      <c r="A146" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B146" s="2">
+        <v>3</v>
+      </c>
+      <c r="C146" s="2">
+        <v>0</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
@@ -6101,11 +6174,21 @@
       <c r="Z146" s="1"/>
     </row>
     <row r="147" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A147" s="1"/>
-      <c r="B147" s="1"/>
-      <c r="C147" s="1"/>
-      <c r="D147" s="1"/>
-      <c r="E147" s="1"/>
+      <c r="A147" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B147" s="2">
+        <v>3</v>
+      </c>
+      <c r="C147" s="2">
+        <v>1</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
@@ -6129,11 +6212,21 @@
       <c r="Z147" s="1"/>
     </row>
     <row r="148" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A148" s="1"/>
-      <c r="B148" s="1"/>
-      <c r="C148" s="1"/>
-      <c r="D148" s="1"/>
-      <c r="E148" s="1"/>
+      <c r="A148" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B148" s="2">
+        <v>4</v>
+      </c>
+      <c r="C148" s="2">
+        <v>0</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
@@ -6157,11 +6250,21 @@
       <c r="Z148" s="1"/>
     </row>
     <row r="149" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A149" s="1"/>
-      <c r="B149" s="1"/>
-      <c r="C149" s="1"/>
-      <c r="D149" s="1"/>
-      <c r="E149" s="1"/>
+      <c r="A149" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B149" s="2">
+        <v>4</v>
+      </c>
+      <c r="C149" s="2">
+        <v>1</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
@@ -6185,11 +6288,21 @@
       <c r="Z149" s="1"/>
     </row>
     <row r="150" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A150" s="1"/>
-      <c r="B150" s="1"/>
-      <c r="C150" s="1"/>
-      <c r="D150" s="1"/>
-      <c r="E150" s="1"/>
+      <c r="A150" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B150" s="2">
+        <v>5</v>
+      </c>
+      <c r="C150" s="2">
+        <v>0</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
@@ -6213,11 +6326,21 @@
       <c r="Z150" s="1"/>
     </row>
     <row r="151" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A151" s="1"/>
-      <c r="B151" s="1"/>
-      <c r="C151" s="1"/>
-      <c r="D151" s="1"/>
-      <c r="E151" s="1"/>
+      <c r="A151" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B151" s="2">
+        <v>5</v>
+      </c>
+      <c r="C151" s="2">
+        <v>0</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
@@ -6241,11 +6364,21 @@
       <c r="Z151" s="1"/>
     </row>
     <row r="152" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
-      <c r="D152" s="1"/>
-      <c r="E152" s="1"/>
+      <c r="A152" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B152" s="2">
+        <v>9</v>
+      </c>
+      <c r="C152" s="2">
+        <v>0</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
@@ -6269,10 +6402,18 @@
       <c r="Z152" s="1"/>
     </row>
     <row r="153" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
-      <c r="C153" s="1"/>
-      <c r="D153" s="1"/>
+      <c r="A153" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B153" s="1">
+        <v>3</v>
+      </c>
+      <c r="C153" s="1">
+        <v>0</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
@@ -29947,9 +30088,9 @@
       <c r="Z998" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E257">
-    <sortCondition ref="A2:A257"/>
-    <sortCondition ref="B2:B257"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E173">
+    <sortCondition ref="A2:A173"/>
+    <sortCondition ref="B2:B173"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
shortened the difficulty to three levels, updated Questions, added and implemented mail-button + small fixes
</commit_message>
<xml_diff>
--- a/SporsmålNidarus.xlsx
+++ b/SporsmålNidarus.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Documents/NTNU/Prosjekt-S22/drikkelek2022-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263723BE-7F42-524E-BBE8-19253B82050B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8544E424-ACBE-8643-9421-05FCBB4A5170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ark2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="186">
   <si>
     <t>Kategori</t>
   </si>
@@ -53,9 +54,6 @@
   </si>
   <si>
     <t>Drikk hvis</t>
-  </si>
-  <si>
-    <t>Drikk hvis du liker betong</t>
   </si>
   <si>
     <t>Drikk hvis du har hatt Skau</t>
@@ -202,9 +200,6 @@
     <t>Hvem er kåtest?</t>
   </si>
   <si>
-    <t>Hvem har hatt sex med flest i dette rommet</t>
-  </si>
-  <si>
     <t>Hvem er best i senga?</t>
   </si>
   <si>
@@ -215,12 +210,6 @@
   </si>
   <si>
     <t xml:space="preserve">Jeg har aldri </t>
-  </si>
-  <si>
-    <t>Jeg ha aldri vært drita med familien</t>
-  </si>
-  <si>
-    <t>Hvem er den beste kysseren</t>
   </si>
   <si>
     <t>Jeg har aldri røyket hasj</t>
@@ -412,9 +401,6 @@
     <t>Hvem koker mest?</t>
   </si>
   <si>
-    <t>memb og memb2 skal ta håndbak</t>
-  </si>
-  <si>
     <t>memb, beskriv ditt beste ligg med tre ord. Ta en skål for hvert ord.</t>
   </si>
   <si>
@@ -431,9 +417,6 @@
   </si>
   <si>
     <t xml:space="preserve">Karaoke!! memb må synge et vers av sin yndlingssang, eller chugge hele drikken sin. </t>
-  </si>
-  <si>
-    <t>memb, gi 2 slurker til den som lukter best</t>
   </si>
   <si>
     <t>memb, gi to slurker til den som snakker mest</t>
@@ -469,9 +452,6 @@
     <t>legg til utfordring</t>
   </si>
   <si>
-    <t>Drikk hvis du har væt i milla</t>
-  </si>
-  <si>
     <t>Personen har gått på folkehøyskole</t>
   </si>
   <si>
@@ -505,10 +485,115 @@
     <t>Hvem har mest kontroll på livet?</t>
   </si>
   <si>
-    <t xml:space="preserve">Drikk hvis du søkte indøk. Chugg hvis du kom inn. </t>
+    <t xml:space="preserve">Drikk hvis du har kjørt elsparkesykkel på fylla. </t>
   </si>
   <si>
-    <t xml:space="preserve">Drikk hvis du har kjørt elsparkesykkel på fylla. </t>
+    <t>Jeg har aldri vært drita med familien</t>
+  </si>
+  <si>
+    <t>memb, gi 2 slurker til den smarteste i rommet</t>
+  </si>
+  <si>
+    <t>Hvem er den beste kysseren?</t>
+  </si>
+  <si>
+    <t>Drikk hvis du har vært i milla</t>
+  </si>
+  <si>
+    <t>Jeg har aldri blitt kjørt hjem av politiet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, la memb2 gå igjennom telefonen din i 30 sek </t>
+  </si>
+  <si>
+    <t>memb, vis memb2 "my eyes only"-bildene dine på snap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pek på den du vil. Personen med færrest pek må drikke. </t>
+  </si>
+  <si>
+    <t>memb, spis et rått egg. Eller chugg.</t>
+  </si>
+  <si>
+    <t>memb, velg hvem som skal spise en teskje kanel</t>
+  </si>
+  <si>
+    <t>Hvem har mest draget?</t>
+  </si>
+  <si>
+    <t>Hvem drikker mest?</t>
+  </si>
+  <si>
+    <t>Hvem er best til å chugge? Personen må chugge drikken sin.</t>
+  </si>
+  <si>
+    <t>Hvem har dårligst smak?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, ta en selfie med alle i rommet og sett det som bakgrunnsbilde. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alle som har bursdag denne måneden kan dele ut 3 slurker. </t>
+  </si>
+  <si>
+    <t>Hvem kommer til å tjene mest?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, fra nå av må du drikke hver gang memb2 stiller et spørsmål. </t>
+  </si>
+  <si>
+    <t>memb, stå på hendene og ta en shot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, ta håndbak med memb2. Vinneren deler ut 4 slurker. </t>
+  </si>
+  <si>
+    <t>memb, hva er de 3 viktigste egenskapene du ser etter i en partner?</t>
+  </si>
+  <si>
+    <t>Hvem får flest superlikes på Tinder?</t>
+  </si>
+  <si>
+    <t>Hvem ville ikke tatt abort?</t>
+  </si>
+  <si>
+    <t>Hvem ville gitt et falskt telefonnummer på byen?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waterfall! memb starter. </t>
+  </si>
+  <si>
+    <t>memb, bytt plass med memb2 og ta en skål</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, illustrer din favoritt-sexstilling med memb2. Eller drikk 4 slurker. </t>
+  </si>
+  <si>
+    <t>Hvem crusher mest?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memb, bytt overdel med en valgfri person, eller drikk 4 slurker. </t>
+  </si>
+  <si>
+    <t>Drikk hvis du holder drikken din nå</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drikk hvis du har kjæreste </t>
+  </si>
+  <si>
+    <t>memb, gjett hvem i rommet som har med kondomer. Ta en slurk for hver gang du gjetter feil.</t>
+  </si>
+  <si>
+    <t>Hvem har høyest bodycount?</t>
+  </si>
+  <si>
+    <t>Personen som onanerte sist kan dele ut 2 slurker</t>
+  </si>
+  <si>
+    <t>memb, gi en slurk til den med høyest standard</t>
+  </si>
+  <si>
+    <t>memb, gi en slurk til den med lavest standard</t>
   </si>
 </sst>
 </file>
@@ -549,12 +634,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -569,12 +660,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266B615A-CB75-A44D-9106-24B2B9F7FAAE}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A144" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -920,7 +1013,6 @@
         <v>4</v>
       </c>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -943,16 +1035,16 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B2" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="1"/>
@@ -978,17 +1070,17 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>97</v>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1"/>
@@ -1018,13 +1110,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1"/>
@@ -1050,19 +1142,19 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="D5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1089,16 +1181,15 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
+      <c r="B6" s="1">
+        <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>153</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1122,19 +1213,19 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2"/>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1162,13 +1253,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1198,13 +1289,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>116</v>
+        <v>179</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1230,19 +1321,19 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="1"/>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1276,8 +1367,9 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>144</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1308,10 +1400,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>157</v>
+        <v>111</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1340,14 +1432,14 @@
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="2">
-        <v>2</v>
+      <c r="B13" s="1">
+        <v>1</v>
       </c>
       <c r="C13" s="2">
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="1"/>
@@ -1373,19 +1465,19 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="1"/>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1413,13 +1505,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1445,19 +1537,19 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="2">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="2"/>
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1484,14 +1576,14 @@
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="2">
-        <v>4</v>
+      <c r="B17" s="1">
+        <v>2</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="1"/>
@@ -1520,14 +1612,14 @@
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="2">
-        <v>5</v>
+      <c r="B18" s="1">
+        <v>2</v>
       </c>
       <c r="C18" s="2">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="1"/>
@@ -1556,14 +1648,14 @@
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="2">
-        <v>5</v>
+      <c r="B19" s="1">
+        <v>2</v>
       </c>
       <c r="C19" s="2">
         <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="1"/>
@@ -1592,8 +1684,8 @@
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="2">
-        <v>6</v>
+      <c r="B20" s="1">
+        <v>2</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -1628,8 +1720,8 @@
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="2">
-        <v>7</v>
+      <c r="B21" s="1">
+        <v>3</v>
       </c>
       <c r="C21" s="2">
         <v>0</v>
@@ -1664,8 +1756,8 @@
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="2">
-        <v>8</v>
+      <c r="B22" s="1">
+        <v>3</v>
       </c>
       <c r="C22" s="2">
         <v>0</v>
@@ -1700,8 +1792,8 @@
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="2">
-        <v>8</v>
+      <c r="B23" s="1">
+        <v>3</v>
       </c>
       <c r="C23" s="2">
         <v>0</v>
@@ -1736,14 +1828,14 @@
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="2">
-        <v>8</v>
+      <c r="B24" s="1">
+        <v>3</v>
       </c>
       <c r="C24" s="2">
         <v>0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="1"/>
@@ -1770,16 +1862,16 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="1"/>
@@ -1806,18 +1898,20 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1842,16 +1936,16 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="1"/>
@@ -1877,19 +1971,19 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="1">
+      <c r="A28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" s="1"/>
+      <c r="D28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="2"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1914,16 +2008,16 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1949,17 +2043,17 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="2">
-        <v>2</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="A30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="5">
         <v>0</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>26</v>
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="1"/>
@@ -1986,16 +2080,16 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="1"/>
@@ -2021,19 +2115,19 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B32" s="2">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2">
+      <c r="A32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="1">
         <v>1</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="2"/>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2058,16 +2152,16 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B33" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="1"/>
@@ -2094,16 +2188,16 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="1"/>
@@ -2130,16 +2224,16 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" s="2">
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="1"/>
@@ -2165,19 +2259,19 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="1">
-        <v>2</v>
-      </c>
-      <c r="C36" s="1">
+      <c r="A36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="2">
         <v>1</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E36" s="1"/>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="2"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2201,19 +2295,19 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="1">
-        <v>2</v>
-      </c>
-      <c r="C37" s="1">
+      <c r="A37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="2">
         <v>1</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E37" s="1"/>
+      <c r="C37" s="2">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="2"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2237,19 +2331,19 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="2">
-        <v>3</v>
-      </c>
-      <c r="C38" s="2">
-        <v>0</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="2"/>
+      <c r="A38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -2273,19 +2367,19 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="2">
-        <v>3</v>
-      </c>
-      <c r="C39" s="2">
-        <v>0</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E39" s="2"/>
+      <c r="A39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -2310,16 +2404,16 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2">
         <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="1"/>
@@ -2346,16 +2440,16 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B41" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C41" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="1"/>
@@ -2382,16 +2476,16 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C42" s="2">
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="1"/>
@@ -2418,16 +2512,16 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B43" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="1"/>
@@ -2454,16 +2548,16 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C44" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="1"/>
@@ -2490,16 +2584,16 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B45" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C45" s="2">
         <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="1"/>
@@ -2526,16 +2620,16 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C46" s="2">
         <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="1"/>
@@ -2562,20 +2656,18 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B47" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C47" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E47" s="2"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -2600,16 +2692,16 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C48" s="2">
         <v>1</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="1"/>
@@ -2636,16 +2728,16 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B49" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C49" s="2">
         <v>1</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="1"/>
@@ -2672,16 +2764,16 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B50" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C50" s="2">
         <v>1</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="1"/>
@@ -2708,16 +2800,16 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B51" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C51" s="2">
         <v>1</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="1"/>
@@ -2744,16 +2836,16 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B52" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C52" s="2">
         <v>1</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="1"/>
@@ -2780,16 +2872,16 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B53" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C53" s="2">
         <v>1</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="1"/>
@@ -2815,19 +2907,19 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B54" s="2">
-        <v>3</v>
-      </c>
-      <c r="C54" s="2">
+      <c r="A54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1">
         <v>0</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E54" s="2"/>
+      <c r="D54" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -2851,17 +2943,17 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>59</v>
+      <c r="A55" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B55" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C55" s="2">
         <v>0</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="1"/>
@@ -2888,16 +2980,16 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B56" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C56" s="2">
         <v>0</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>63</v>
+        <v>150</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="1"/>
@@ -2924,16 +3016,16 @@
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B57" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="1"/>
@@ -2960,16 +3052,16 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C58" s="2">
         <v>0</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="1"/>
@@ -2996,16 +3088,16 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B59" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C59" s="2">
         <v>0</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="1"/>
@@ -3032,16 +3124,16 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B60" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C60" s="2">
         <v>0</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="1"/>
@@ -3068,16 +3160,16 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B61" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C61" s="2">
         <v>0</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="1"/>
@@ -3103,17 +3195,17 @@
       <c r="Z61" s="1"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>59</v>
+      <c r="A62" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B62" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C62" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" s="1"/>
@@ -3140,16 +3232,16 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B63" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C63" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>130</v>
+        <v>61</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="1"/>
@@ -3176,16 +3268,16 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="B64" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C64" s="2">
         <v>0</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="1"/>
@@ -3212,7 +3304,7 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B65" s="2">
         <v>1</v>
@@ -3221,7 +3313,7 @@
         <v>0</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="1"/>
@@ -3248,7 +3340,7 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B66" s="2">
         <v>1</v>
@@ -3257,7 +3349,7 @@
         <v>0</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" s="1"/>
@@ -3284,7 +3376,7 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B67" s="2">
         <v>1</v>
@@ -3293,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="1"/>
@@ -3320,7 +3412,7 @@
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B68" s="2">
         <v>1</v>
@@ -3329,7 +3421,7 @@
         <v>0</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="1"/>
@@ -3356,7 +3448,7 @@
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B69" s="2">
         <v>1</v>
@@ -3365,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" s="1"/>
@@ -3392,7 +3484,7 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B70" s="2">
         <v>1</v>
@@ -3401,7 +3493,7 @@
         <v>0</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="1"/>
@@ -3428,7 +3520,7 @@
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B71" s="2">
         <v>1</v>
@@ -3437,7 +3529,7 @@
         <v>0</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" s="1"/>
@@ -3464,7 +3556,7 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B72" s="2">
         <v>1</v>
@@ -3473,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" s="1"/>
@@ -3500,7 +3592,7 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B73" s="2">
         <v>1</v>
@@ -3509,7 +3601,7 @@
         <v>0</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="1"/>
@@ -3536,7 +3628,7 @@
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="B74" s="2">
         <v>1</v>
@@ -3545,7 +3637,7 @@
         <v>0</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" s="1"/>
@@ -3572,16 +3664,16 @@
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B75" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E75" s="2"/>
       <c r="F75" s="1"/>
@@ -3608,16 +3700,16 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B76" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76" s="2">
         <v>0</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" s="1"/>
@@ -3643,19 +3735,19 @@
       <c r="Z76" s="1"/>
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B77" s="2">
+      <c r="A77" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1">
         <v>1</v>
       </c>
-      <c r="C77" s="2">
-        <v>0</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E77" s="2"/>
+      <c r="D77" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
@@ -3679,19 +3771,19 @@
       <c r="Z77" s="1"/>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B78" s="2">
-        <v>1</v>
-      </c>
-      <c r="C78" s="2">
+      <c r="A78" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B78" s="1">
         <v>0</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E78" s="2"/>
+      <c r="C78" s="1">
+        <v>0</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
@@ -3716,16 +3808,16 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B79" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C79" s="2">
         <v>0</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" s="1"/>
@@ -3752,18 +3844,18 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B80" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80" s="2">
         <v>0</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E80" s="2"/>
+        <v>151</v>
+      </c>
+      <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
@@ -3787,17 +3879,17 @@
       <c r="Z80" s="1"/>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B81" s="2">
-        <v>1</v>
-      </c>
-      <c r="C81" s="2">
+      <c r="A81" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B81" s="1">
         <v>0</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>132</v>
+      <c r="C81" s="1">
+        <v>0</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -3822,9 +3914,9 @@
       <c r="Y81" s="1"/>
       <c r="Z81" s="1"/>
     </row>
-    <row r="82" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B82" s="2">
         <v>1</v>
@@ -3832,10 +3924,10 @@
       <c r="C82" s="2">
         <v>0</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E82" s="1"/>
+      <c r="D82" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E82" s="2"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
@@ -3859,19 +3951,19 @@
       <c r="Z82" s="1"/>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B83" s="1">
+      <c r="A83" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B83" s="2">
         <v>1</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C83" s="2">
         <v>0</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E83" s="1"/>
+      <c r="D83" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E83" s="2"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
@@ -3895,19 +3987,19 @@
       <c r="Z83" s="1"/>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B84" s="1">
+      <c r="A84" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B84" s="2">
         <v>1</v>
       </c>
-      <c r="C84" s="1">
+      <c r="C84" s="2">
         <v>0</v>
       </c>
-      <c r="D84" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E84" s="1"/>
+      <c r="D84" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E84" s="2"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
@@ -3931,19 +4023,19 @@
       <c r="Z84" s="1"/>
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B85" s="1">
+      <c r="A85" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B85" s="2">
         <v>1</v>
       </c>
-      <c r="C85" s="1">
+      <c r="C85" s="2">
         <v>0</v>
       </c>
-      <c r="D85" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E85" s="1"/>
+      <c r="D85" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E85" s="2"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
@@ -3966,18 +4058,18 @@
       <c r="Y85" s="1"/>
       <c r="Z85" s="1"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B86" s="1">
+    <row r="86" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B86" s="2">
         <v>1</v>
       </c>
-      <c r="C86" s="1">
+      <c r="C86" s="2">
         <v>0</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>142</v>
+      <c r="D86" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -4004,7 +4096,7 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B87" s="1">
         <v>1</v>
@@ -4013,7 +4105,7 @@
         <v>0</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -4040,7 +4132,7 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B88" s="1">
         <v>1</v>
@@ -4049,7 +4141,7 @@
         <v>0</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -4075,19 +4167,21 @@
       <c r="Z88" s="1"/>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>42</v>
+      <c r="A89" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B89" s="1">
         <v>1</v>
       </c>
-      <c r="C89" s="1">
+      <c r="C89" s="2">
         <v>0</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E89" s="1"/>
+      <c r="D89" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
@@ -4112,7 +4206,7 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B90" s="1">
         <v>1</v>
@@ -4121,7 +4215,7 @@
         <v>0</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
@@ -4146,21 +4240,18 @@
       <c r="Y90" s="1"/>
       <c r="Z90" s="1"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A91" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B91" s="2">
-        <v>2</v>
-      </c>
-      <c r="C91" s="2">
+    <row r="91" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B91" s="1">
+        <v>1</v>
+      </c>
+      <c r="C91" s="1">
         <v>0</v>
       </c>
-      <c r="D91" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>43</v>
+      <c r="D91" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
@@ -4184,20 +4275,19 @@
       <c r="Y91" s="1"/>
       <c r="Z91" s="1"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B92" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C92" s="1">
         <v>0</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E92" s="1"/>
+      <c r="D92" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
@@ -4222,16 +4312,16 @@
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B93" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C93" s="1">
         <v>0</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -4256,19 +4346,20 @@
       <c r="Y93" s="1"/>
       <c r="Z93" s="1"/>
     </row>
-    <row r="94" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B94" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C94" s="1">
         <v>0</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="D94" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
@@ -4291,19 +4382,20 @@
       <c r="Y94" s="1"/>
       <c r="Z94" s="1"/>
     </row>
-    <row r="95" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B95" s="1">
-        <v>2</v>
-      </c>
-      <c r="C95" s="1">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B95" s="2">
+        <v>1</v>
+      </c>
+      <c r="C95" s="2">
         <v>0</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="D95" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
@@ -4327,17 +4419,17 @@
       <c r="Z95" s="1"/>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B96" s="1">
-        <v>2</v>
-      </c>
-      <c r="C96" s="1">
+      <c r="A96" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B96" s="2">
+        <v>1</v>
+      </c>
+      <c r="C96" s="2">
         <v>0</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>150</v>
+      <c r="D96" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -4364,16 +4456,16 @@
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B97" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C97" s="1">
         <v>0</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -4400,16 +4492,16 @@
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B98" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C98" s="1">
         <v>0</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>127</v>
+        <v>175</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -4436,16 +4528,16 @@
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B99" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C99" s="1">
         <v>0</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -4471,19 +4563,19 @@
       <c r="Z99" s="1"/>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B100" s="2">
-        <v>4</v>
-      </c>
-      <c r="C100" s="2">
-        <v>0</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E100" s="2"/>
+      <c r="A100" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B100" s="1">
+        <v>1</v>
+      </c>
+      <c r="C100" s="1">
+        <v>2</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
@@ -4507,19 +4599,19 @@
       <c r="Z100" s="1"/>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B101" s="2">
-        <v>4</v>
-      </c>
-      <c r="C101" s="2">
-        <v>0</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E101" s="2"/>
+      <c r="A101" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B101" s="1">
+        <v>1</v>
+      </c>
+      <c r="C101" s="1">
+        <v>1</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
@@ -4543,19 +4635,19 @@
       <c r="Z101" s="1"/>
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A102" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B102" s="2">
-        <v>4</v>
-      </c>
-      <c r="C102" s="2">
-        <v>0</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E102" s="2"/>
+      <c r="A102" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B102" s="1">
+        <v>1</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
@@ -4579,19 +4671,19 @@
       <c r="Z102" s="1"/>
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B103" s="2">
-        <v>4</v>
-      </c>
-      <c r="C103" s="2">
-        <v>0</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E103" s="2"/>
+      <c r="A103" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B103" s="1">
+        <v>1</v>
+      </c>
+      <c r="C103" s="1">
+        <v>1</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
@@ -4615,19 +4707,19 @@
       <c r="Z103" s="1"/>
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A104" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B104" s="2">
-        <v>4</v>
-      </c>
-      <c r="C104" s="2">
+      <c r="A104" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B104" s="1">
+        <v>2</v>
+      </c>
+      <c r="C104" s="1">
         <v>0</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E104" s="2"/>
+      <c r="D104" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E104" s="1"/>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
@@ -4651,17 +4743,17 @@
       <c r="Z104" s="1"/>
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B105" s="2">
-        <v>4</v>
-      </c>
-      <c r="C105" s="2">
+      <c r="A105" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B105" s="1">
+        <v>2</v>
+      </c>
+      <c r="C105" s="1">
         <v>0</v>
       </c>
-      <c r="D105" s="2" t="s">
-        <v>104</v>
+      <c r="D105" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
@@ -4688,16 +4780,16 @@
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B106" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C106" s="1">
         <v>0</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
@@ -4723,19 +4815,19 @@
       <c r="Z106" s="1"/>
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A107" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B107" s="2">
-        <v>5</v>
-      </c>
-      <c r="C107" s="2">
+      <c r="A107" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B107" s="1">
+        <v>2</v>
+      </c>
+      <c r="C107" s="1">
         <v>0</v>
       </c>
-      <c r="D107" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E107" s="2"/>
+      <c r="D107" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E107" s="1"/>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
@@ -4759,19 +4851,19 @@
       <c r="Z107" s="1"/>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A108" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B108" s="2">
-        <v>5</v>
-      </c>
-      <c r="C108" s="2">
+      <c r="A108" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B108" s="1">
+        <v>2</v>
+      </c>
+      <c r="C108" s="1">
         <v>0</v>
       </c>
-      <c r="D108" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E108" s="2"/>
+      <c r="D108" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
@@ -4796,16 +4888,16 @@
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B109" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C109" s="1">
         <v>0</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -4832,16 +4924,16 @@
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B110" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C110" s="1">
         <v>0</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
@@ -4867,19 +4959,19 @@
       <c r="Z110" s="1"/>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A111" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B111" s="2">
-        <v>6</v>
-      </c>
-      <c r="C111" s="2">
+      <c r="A111" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B111" s="1">
+        <v>2</v>
+      </c>
+      <c r="C111" s="1">
         <v>0</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E111" s="2"/>
+      <c r="D111" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E111" s="1"/>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
@@ -4904,16 +4996,16 @@
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B112" s="2">
-        <v>6</v>
+        <v>41</v>
+      </c>
+      <c r="B112" s="1">
+        <v>2</v>
       </c>
       <c r="C112" s="2">
         <v>0</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" s="1"/>
@@ -4940,16 +5032,16 @@
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B113" s="2">
-        <v>6</v>
+        <v>41</v>
+      </c>
+      <c r="B113" s="1">
+        <v>2</v>
       </c>
       <c r="C113" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113" s="1"/>
@@ -4976,16 +5068,16 @@
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B114" s="2">
-        <v>6</v>
+        <v>41</v>
+      </c>
+      <c r="B114" s="1">
+        <v>2</v>
       </c>
       <c r="C114" s="2">
         <v>0</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" s="1"/>
@@ -5011,19 +5103,19 @@
       <c r="Z114" s="1"/>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A115" s="1" t="s">
-        <v>42</v>
+      <c r="A115" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B115" s="1">
-        <v>6</v>
-      </c>
-      <c r="C115" s="1">
+        <v>3</v>
+      </c>
+      <c r="C115" s="2">
         <v>0</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E115" s="1"/>
+      <c r="D115" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E115" s="2"/>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
@@ -5047,19 +5139,19 @@
       <c r="Z115" s="1"/>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>42</v>
+      <c r="A116" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B116" s="1">
-        <v>6</v>
-      </c>
-      <c r="C116" s="1">
+        <v>2</v>
+      </c>
+      <c r="C116" s="2">
         <v>0</v>
       </c>
-      <c r="D116" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E116" s="1"/>
+      <c r="D116" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E116" s="2"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
@@ -5084,18 +5176,18 @@
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B117" s="2">
-        <v>7</v>
+        <v>41</v>
+      </c>
+      <c r="B117" s="1">
+        <v>2</v>
       </c>
       <c r="C117" s="2">
         <v>0</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E117" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
@@ -5119,19 +5211,19 @@
       <c r="Z117" s="1"/>
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A118" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B118" s="2">
-        <v>8</v>
-      </c>
-      <c r="C118" s="2">
+      <c r="A118" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B118" s="1">
+        <v>2</v>
+      </c>
+      <c r="C118" s="1">
         <v>0</v>
       </c>
-      <c r="D118" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E118" s="2"/>
+      <c r="D118" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E118" s="1"/>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
@@ -5155,19 +5247,19 @@
       <c r="Z118" s="1"/>
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A119" s="1" t="s">
-        <v>42</v>
+      <c r="A119" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B119" s="1">
-        <v>8</v>
-      </c>
-      <c r="C119" s="1">
+        <v>2</v>
+      </c>
+      <c r="C119" s="2">
         <v>0</v>
       </c>
-      <c r="D119" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E119" s="1"/>
+      <c r="D119" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E119" s="2"/>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
@@ -5192,16 +5284,16 @@
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B120" s="2">
-        <v>9</v>
+        <v>41</v>
+      </c>
+      <c r="B120" s="1">
+        <v>2</v>
       </c>
       <c r="C120" s="2">
         <v>0</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E120" s="2"/>
       <c r="F120" s="1"/>
@@ -5227,19 +5319,19 @@
       <c r="Z120" s="1"/>
     </row>
     <row r="121" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A121" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B121" s="2">
-        <v>9</v>
-      </c>
-      <c r="C121" s="2">
+      <c r="A121" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B121" s="1">
+        <v>2</v>
+      </c>
+      <c r="C121" s="1">
         <v>0</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E121" s="2"/>
+      <c r="D121" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E121" s="1"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
@@ -5263,19 +5355,19 @@
       <c r="Z121" s="1"/>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A122" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B122" s="2">
-        <v>9</v>
-      </c>
-      <c r="C122" s="2">
+      <c r="A122" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B122" s="1">
+        <v>2</v>
+      </c>
+      <c r="C122" s="1">
         <v>0</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E122" s="2"/>
+      <c r="D122" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E122" s="1"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
@@ -5300,16 +5392,16 @@
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B123" s="2">
-        <v>10</v>
+        <v>41</v>
+      </c>
+      <c r="B123" s="1">
+        <v>2</v>
       </c>
       <c r="C123" s="2">
         <v>0</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E123" s="2"/>
       <c r="F123" s="1"/>
@@ -5335,19 +5427,19 @@
       <c r="Z123" s="1"/>
     </row>
     <row r="124" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
-        <v>42</v>
+      <c r="A124" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B124" s="1">
-        <v>10</v>
-      </c>
-      <c r="C124" s="1">
+        <v>2</v>
+      </c>
+      <c r="C124" s="2">
         <v>0</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E124" s="1"/>
+      <c r="D124" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E124" s="2"/>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
@@ -5372,16 +5464,16 @@
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B125" s="2">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B125" s="1">
+        <v>2</v>
       </c>
       <c r="C125" s="2">
         <v>1</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125" s="1"/>
@@ -5408,16 +5500,16 @@
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B126" s="2">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B126" s="1">
+        <v>2</v>
       </c>
       <c r="C126" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126" s="1"/>
@@ -5443,19 +5535,19 @@
       <c r="Z126" s="1"/>
     </row>
     <row r="127" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A127" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B127" s="2">
-        <v>1</v>
-      </c>
-      <c r="C127" s="2">
-        <v>1</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E127" s="2"/>
+      <c r="A127" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B127" s="1">
+        <v>2</v>
+      </c>
+      <c r="C127" s="1">
+        <v>0</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
@@ -5479,19 +5571,19 @@
       <c r="Z127" s="1"/>
     </row>
     <row r="128" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A128" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B128" s="2">
-        <v>1</v>
-      </c>
-      <c r="C128" s="2">
-        <v>1</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E128" s="2"/>
+      <c r="A128" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B128" s="1">
+        <v>2</v>
+      </c>
+      <c r="C128" s="1">
+        <v>0</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
@@ -5516,18 +5608,18 @@
     </row>
     <row r="129" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="B129" s="1">
-        <v>1</v>
-      </c>
-      <c r="C129" s="1">
-        <v>1</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E129" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C129" s="2">
+        <v>0</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E129" s="2"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
@@ -5551,17 +5643,17 @@
       <c r="Z129" s="1"/>
     </row>
     <row r="130" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A130" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B130" s="2">
-        <v>1</v>
+      <c r="A130" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B130" s="1">
+        <v>2</v>
       </c>
       <c r="C130" s="2">
-        <v>1</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>106</v>
+        <v>0</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -5587,18 +5679,19 @@
       <c r="Z130" s="1"/>
     </row>
     <row r="131" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A131" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B131" s="2">
-        <v>1</v>
-      </c>
-      <c r="C131" s="2">
+      <c r="A131" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B131" s="1">
+        <v>2</v>
+      </c>
+      <c r="C131" s="1">
         <v>0</v>
       </c>
-      <c r="D131" s="2" t="s">
-        <v>145</v>
-      </c>
+      <c r="D131" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
@@ -5622,19 +5715,19 @@
       <c r="Z131" s="1"/>
     </row>
     <row r="132" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A132" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B132" s="2">
+      <c r="A132" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B132" s="1">
         <v>2</v>
       </c>
-      <c r="C132" s="2">
-        <v>1</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E132" s="2"/>
+      <c r="C132" s="1">
+        <v>0</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E132" s="1"/>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
@@ -5659,16 +5752,16 @@
     </row>
     <row r="133" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B133" s="2">
-        <v>2</v>
+        <v>41</v>
+      </c>
+      <c r="B133" s="1">
+        <v>3</v>
       </c>
       <c r="C133" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="E133" s="2"/>
       <c r="F133" s="1"/>
@@ -5694,21 +5787,19 @@
       <c r="Z133" s="1"/>
     </row>
     <row r="134" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A134" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B134" s="2">
-        <v>1</v>
-      </c>
-      <c r="C134" s="2">
+      <c r="A134" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B134" s="1">
+        <v>3</v>
+      </c>
+      <c r="C134" s="1">
         <v>0</v>
       </c>
-      <c r="D134" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="D134" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
@@ -5733,20 +5824,18 @@
     </row>
     <row r="135" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B135" s="2">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B135" s="1">
+        <v>3</v>
       </c>
       <c r="C135" s="2">
         <v>0</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="E135" s="2"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
@@ -5771,20 +5860,18 @@
     </row>
     <row r="136" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B136" s="2">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B136" s="1">
+        <v>3</v>
       </c>
       <c r="C136" s="2">
         <v>0</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E136" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="E136" s="2"/>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
@@ -5809,20 +5896,18 @@
     </row>
     <row r="137" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B137" s="2">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="B137" s="1">
+        <v>3</v>
       </c>
       <c r="C137" s="2">
         <v>0</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E137" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="E137" s="2"/>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
@@ -5846,19 +5931,19 @@
       <c r="Z137" s="1"/>
     </row>
     <row r="138" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
-        <v>50</v>
+      <c r="A138" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B138" s="1">
-        <v>1</v>
-      </c>
-      <c r="C138" s="1">
+        <v>3</v>
+      </c>
+      <c r="C138" s="2">
         <v>0</v>
       </c>
-      <c r="D138" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E138" s="1"/>
+      <c r="D138" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E138" s="2"/>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
@@ -5883,16 +5968,16 @@
     </row>
     <row r="139" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B139" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C139" s="1">
         <v>0</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -5919,16 +6004,16 @@
     </row>
     <row r="140" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B140" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C140" s="1">
         <v>0</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>109</v>
+        <v>158</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
@@ -5955,16 +6040,16 @@
     </row>
     <row r="141" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B141" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C141" s="1">
         <v>0</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
@@ -5991,16 +6076,16 @@
     </row>
     <row r="142" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B142" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C142" s="1">
         <v>0</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
@@ -6027,16 +6112,16 @@
     </row>
     <row r="143" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B143" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C143" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>124</v>
+        <v>168</v>
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
@@ -6063,16 +6148,16 @@
     </row>
     <row r="144" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B144" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C144" s="1">
         <v>0</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
@@ -6099,20 +6184,18 @@
     </row>
     <row r="145" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B145" s="2">
-        <v>2</v>
+        <v>101</v>
+      </c>
+      <c r="B145" s="1">
+        <v>0</v>
       </c>
       <c r="C145" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E145" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E145" s="2"/>
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
@@ -6137,20 +6220,18 @@
     </row>
     <row r="146" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B146" s="2">
-        <v>3</v>
+        <v>101</v>
+      </c>
+      <c r="B146" s="1">
+        <v>0</v>
       </c>
       <c r="C146" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E146" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E146" s="2"/>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
@@ -6175,20 +6256,18 @@
     </row>
     <row r="147" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B147" s="2">
-        <v>3</v>
+        <v>101</v>
+      </c>
+      <c r="B147" s="1">
+        <v>0</v>
       </c>
       <c r="C147" s="2">
         <v>1</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E147" s="2"/>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
@@ -6213,20 +6292,18 @@
     </row>
     <row r="148" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B148" s="2">
-        <v>4</v>
+        <v>101</v>
+      </c>
+      <c r="B148" s="1">
+        <v>0</v>
       </c>
       <c r="C148" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E148" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="E148" s="2"/>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
@@ -6251,20 +6328,18 @@
     </row>
     <row r="149" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B149" s="2">
-        <v>4</v>
-      </c>
-      <c r="C149" s="2">
+        <v>101</v>
+      </c>
+      <c r="B149" s="1">
+        <v>0</v>
+      </c>
+      <c r="C149" s="1">
         <v>1</v>
       </c>
-      <c r="D149" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E149" s="2" t="s">
-        <v>58</v>
-      </c>
+      <c r="D149" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E149" s="1"/>
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
@@ -6289,20 +6364,18 @@
     </row>
     <row r="150" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B150" s="2">
-        <v>5</v>
+        <v>101</v>
+      </c>
+      <c r="B150" s="1">
+        <v>0</v>
       </c>
       <c r="C150" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E150" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E150" s="1"/>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
@@ -6327,19 +6400,16 @@
     </row>
     <row r="151" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B151" s="2">
-        <v>5</v>
+        <v>101</v>
+      </c>
+      <c r="B151" s="1">
+        <v>0</v>
       </c>
       <c r="C151" s="2">
         <v>0</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
@@ -6365,20 +6435,18 @@
     </row>
     <row r="152" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B152" s="2">
-        <v>9</v>
+        <v>101</v>
+      </c>
+      <c r="B152" s="1">
+        <v>0</v>
       </c>
       <c r="C152" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E152" s="2" t="s">
-        <v>85</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="E152" s="2"/>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
@@ -6402,19 +6470,19 @@
       <c r="Z152" s="1"/>
     </row>
     <row r="153" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A153" s="1" t="s">
-        <v>153</v>
+      <c r="A153" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="B153" s="1">
-        <v>3</v>
-      </c>
-      <c r="C153" s="1">
-        <v>0</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E153" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C153" s="2">
+        <v>1</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E153" s="2"/>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
@@ -6438,10 +6506,18 @@
       <c r="Z153" s="1"/>
     </row>
     <row r="154" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A154" s="1"/>
-      <c r="B154" s="1"/>
-      <c r="C154" s="1"/>
-      <c r="D154" s="1"/>
+      <c r="A154" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B154" s="1">
+        <v>0</v>
+      </c>
+      <c r="C154" s="1">
+        <v>0</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
@@ -6466,10 +6542,18 @@
       <c r="Z154" s="1"/>
     </row>
     <row r="155" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A155" s="1"/>
-      <c r="B155" s="1"/>
-      <c r="C155" s="1"/>
-      <c r="D155" s="1"/>
+      <c r="A155" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B155" s="1">
+        <v>0</v>
+      </c>
+      <c r="C155" s="1">
+        <v>0</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
@@ -6494,10 +6578,18 @@
       <c r="Z155" s="1"/>
     </row>
     <row r="156" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A156" s="1"/>
-      <c r="B156" s="1"/>
-      <c r="C156" s="1"/>
-      <c r="D156" s="1"/>
+      <c r="A156" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B156" s="6">
+        <v>0</v>
+      </c>
+      <c r="C156" s="6">
+        <v>0</v>
+      </c>
+      <c r="D156" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
       <c r="G156" s="1"/>
@@ -6522,10 +6614,18 @@
       <c r="Z156" s="1"/>
     </row>
     <row r="157" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A157" s="1"/>
-      <c r="B157" s="1"/>
-      <c r="C157" s="1"/>
-      <c r="D157" s="1"/>
+      <c r="A157" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B157" s="1">
+        <v>0</v>
+      </c>
+      <c r="C157" s="1">
+        <v>0</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
@@ -6550,10 +6650,18 @@
       <c r="Z157" s="1"/>
     </row>
     <row r="158" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A158" s="1"/>
-      <c r="B158" s="1"/>
-      <c r="C158" s="1"/>
-      <c r="D158" s="1"/>
+      <c r="A158" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B158" s="1">
+        <v>0</v>
+      </c>
+      <c r="C158" s="1">
+        <v>0</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
@@ -6578,11 +6686,11 @@
       <c r="Z158" s="1"/>
     </row>
     <row r="159" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A159" s="1"/>
+      <c r="A159" s="2"/>
       <c r="B159" s="1"/>
-      <c r="C159" s="1"/>
-      <c r="D159" s="1"/>
-      <c r="E159" s="1"/>
+      <c r="C159" s="2"/>
+      <c r="D159" s="2"/>
+      <c r="E159" s="2"/>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
@@ -6634,10 +6742,10 @@
       <c r="Z160" s="1"/>
     </row>
     <row r="161" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A161" s="1"/>
-      <c r="B161" s="1"/>
-      <c r="C161" s="1"/>
-      <c r="D161" s="1"/>
+      <c r="A161" s="6"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="6"/>
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
@@ -6690,11 +6798,11 @@
       <c r="Z162" s="1"/>
     </row>
     <row r="163" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A163" s="1"/>
+      <c r="A163" s="2"/>
       <c r="B163" s="1"/>
-      <c r="C163" s="1"/>
-      <c r="D163" s="1"/>
-      <c r="E163" s="1"/>
+      <c r="C163" s="2"/>
+      <c r="D163" s="2"/>
+      <c r="E163" s="2"/>
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
@@ -6718,11 +6826,11 @@
       <c r="Z163" s="1"/>
     </row>
     <row r="164" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A164" s="1"/>
+      <c r="A164" s="2"/>
       <c r="B164" s="1"/>
-      <c r="C164" s="1"/>
-      <c r="D164" s="1"/>
-      <c r="E164" s="1"/>
+      <c r="C164" s="2"/>
+      <c r="D164" s="2"/>
+      <c r="E164" s="2"/>
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
@@ -6746,11 +6854,11 @@
       <c r="Z164" s="1"/>
     </row>
     <row r="165" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A165" s="1"/>
+      <c r="A165" s="2"/>
       <c r="B165" s="1"/>
-      <c r="C165" s="1"/>
-      <c r="D165" s="1"/>
-      <c r="E165" s="1"/>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
+      <c r="E165" s="2"/>
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
@@ -6830,11 +6938,11 @@
       <c r="Z167" s="1"/>
     </row>
     <row r="168" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A168" s="1"/>
+      <c r="A168" s="2"/>
       <c r="B168" s="1"/>
-      <c r="C168" s="1"/>
-      <c r="D168" s="1"/>
-      <c r="E168" s="1"/>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="2"/>
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
@@ -6858,11 +6966,11 @@
       <c r="Z168" s="1"/>
     </row>
     <row r="169" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A169" s="1"/>
+      <c r="A169" s="2"/>
       <c r="B169" s="1"/>
-      <c r="C169" s="1"/>
-      <c r="D169" s="1"/>
-      <c r="E169" s="1"/>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
+      <c r="E169" s="2"/>
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
@@ -6944,7 +7052,6 @@
     <row r="172" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
-      <c r="C172" s="1"/>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
       <c r="F172" s="1"/>
@@ -7082,11 +7189,11 @@
       <c r="Z176" s="1"/>
     </row>
     <row r="177" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A177" s="1"/>
+      <c r="A177" s="2"/>
       <c r="B177" s="1"/>
-      <c r="C177" s="1"/>
-      <c r="D177" s="1"/>
-      <c r="E177" s="1"/>
+      <c r="C177" s="2"/>
+      <c r="D177" s="2"/>
+      <c r="E177" s="2"/>
       <c r="F177" s="1"/>
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
@@ -7110,11 +7217,11 @@
       <c r="Z177" s="1"/>
     </row>
     <row r="178" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A178" s="1"/>
+      <c r="A178" s="2"/>
       <c r="B178" s="1"/>
-      <c r="C178" s="1"/>
-      <c r="D178" s="1"/>
-      <c r="E178" s="1"/>
+      <c r="C178" s="2"/>
+      <c r="D178" s="2"/>
+      <c r="E178" s="2"/>
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
@@ -7138,11 +7245,11 @@
       <c r="Z178" s="1"/>
     </row>
     <row r="179" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A179" s="1"/>
+      <c r="A179" s="2"/>
       <c r="B179" s="1"/>
-      <c r="C179" s="1"/>
-      <c r="D179" s="1"/>
-      <c r="E179" s="1"/>
+      <c r="C179" s="2"/>
+      <c r="D179" s="2"/>
+      <c r="E179" s="2"/>
       <c r="F179" s="1"/>
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
@@ -7166,11 +7273,11 @@
       <c r="Z179" s="1"/>
     </row>
     <row r="180" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A180" s="1"/>
+      <c r="A180" s="2"/>
       <c r="B180" s="1"/>
-      <c r="C180" s="1"/>
-      <c r="D180" s="1"/>
-      <c r="E180" s="1"/>
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
+      <c r="E180" s="2"/>
       <c r="F180" s="1"/>
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
@@ -7194,11 +7301,11 @@
       <c r="Z180" s="1"/>
     </row>
     <row r="181" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A181" s="1"/>
+      <c r="A181" s="2"/>
       <c r="B181" s="1"/>
-      <c r="C181" s="1"/>
-      <c r="D181" s="1"/>
-      <c r="E181" s="1"/>
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
+      <c r="E181" s="2"/>
       <c r="F181" s="1"/>
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
@@ -7278,11 +7385,11 @@
       <c r="Z183" s="1"/>
     </row>
     <row r="184" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A184" s="1"/>
+      <c r="A184" s="2"/>
       <c r="B184" s="1"/>
-      <c r="C184" s="1"/>
-      <c r="D184" s="1"/>
-      <c r="E184" s="1"/>
+      <c r="C184" s="2"/>
+      <c r="D184" s="2"/>
+      <c r="E184" s="2"/>
       <c r="F184" s="1"/>
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
@@ -7337,7 +7444,6 @@
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
-      <c r="D186" s="1"/>
       <c r="E186" s="1"/>
       <c r="F186" s="1"/>
       <c r="G186" s="1"/>
@@ -7365,7 +7471,6 @@
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
-      <c r="D187" s="1"/>
       <c r="E187" s="1"/>
       <c r="F187" s="1"/>
       <c r="G187" s="1"/>
@@ -7446,18 +7551,6 @@
       <c r="Z189" s="1"/>
     </row>
     <row r="190" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A190" s="1"/>
-      <c r="B190" s="1"/>
-      <c r="C190" s="1"/>
-      <c r="D190" s="1"/>
-      <c r="E190" s="1"/>
-      <c r="F190" s="1"/>
-      <c r="G190" s="1"/>
-      <c r="H190" s="1"/>
-      <c r="I190" s="1"/>
-      <c r="J190" s="1"/>
-      <c r="K190" s="1"/>
-      <c r="L190" s="1"/>
       <c r="M190" s="1"/>
       <c r="N190" s="1"/>
       <c r="O190" s="1"/>
@@ -11114,11 +11207,6 @@
       <c r="Z320" s="1"/>
     </row>
     <row r="321" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A321" s="1"/>
-      <c r="B321" s="1"/>
-      <c r="C321" s="1"/>
-      <c r="D321" s="1"/>
-      <c r="E321" s="1"/>
       <c r="F321" s="1"/>
       <c r="G321" s="1"/>
       <c r="H321" s="1"/>
@@ -11142,11 +11230,6 @@
       <c r="Z321" s="1"/>
     </row>
     <row r="322" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A322" s="1"/>
-      <c r="B322" s="1"/>
-      <c r="C322" s="1"/>
-      <c r="D322" s="1"/>
-      <c r="E322" s="1"/>
       <c r="F322" s="1"/>
       <c r="G322" s="1"/>
       <c r="H322" s="1"/>
@@ -11226,6 +11309,11 @@
       <c r="Z324" s="1"/>
     </row>
     <row r="325" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A325" s="1"/>
+      <c r="B325" s="1"/>
+      <c r="C325" s="1"/>
+      <c r="D325" s="1"/>
+      <c r="E325" s="1"/>
       <c r="F325" s="1"/>
       <c r="G325" s="1"/>
       <c r="H325" s="1"/>
@@ -11249,6 +11337,11 @@
       <c r="Z325" s="1"/>
     </row>
     <row r="326" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A326" s="1"/>
+      <c r="B326" s="1"/>
+      <c r="C326" s="1"/>
+      <c r="D326" s="1"/>
+      <c r="E326" s="1"/>
       <c r="F326" s="1"/>
       <c r="G326" s="1"/>
       <c r="H326" s="1"/>
@@ -29975,124 +30068,516 @@
       <c r="Y994" s="1"/>
       <c r="Z994" s="1"/>
     </row>
-    <row r="995" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A995" s="1"/>
-      <c r="B995" s="1"/>
-      <c r="C995" s="1"/>
-      <c r="D995" s="1"/>
-      <c r="E995" s="1"/>
-      <c r="F995" s="1"/>
-      <c r="G995" s="1"/>
-      <c r="H995" s="1"/>
-      <c r="I995" s="1"/>
-      <c r="J995" s="1"/>
-      <c r="K995" s="1"/>
-      <c r="L995" s="1"/>
-      <c r="M995" s="1"/>
-      <c r="N995" s="1"/>
-      <c r="O995" s="1"/>
-      <c r="P995" s="1"/>
-      <c r="Q995" s="1"/>
-      <c r="R995" s="1"/>
-      <c r="S995" s="1"/>
-      <c r="T995" s="1"/>
-      <c r="U995" s="1"/>
-      <c r="V995" s="1"/>
-      <c r="W995" s="1"/>
-      <c r="X995" s="1"/>
-      <c r="Y995" s="1"/>
-      <c r="Z995" s="1"/>
-    </row>
-    <row r="996" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A996" s="1"/>
-      <c r="B996" s="1"/>
-      <c r="C996" s="1"/>
-      <c r="D996" s="1"/>
-      <c r="E996" s="1"/>
-      <c r="F996" s="1"/>
-      <c r="G996" s="1"/>
-      <c r="H996" s="1"/>
-      <c r="I996" s="1"/>
-      <c r="J996" s="1"/>
-      <c r="K996" s="1"/>
-      <c r="L996" s="1"/>
-      <c r="M996" s="1"/>
-      <c r="N996" s="1"/>
-      <c r="O996" s="1"/>
-      <c r="P996" s="1"/>
-      <c r="Q996" s="1"/>
-      <c r="R996" s="1"/>
-      <c r="S996" s="1"/>
-      <c r="T996" s="1"/>
-      <c r="U996" s="1"/>
-      <c r="V996" s="1"/>
-      <c r="W996" s="1"/>
-      <c r="X996" s="1"/>
-      <c r="Y996" s="1"/>
-      <c r="Z996" s="1"/>
-    </row>
-    <row r="997" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A997" s="1"/>
-      <c r="B997" s="1"/>
-      <c r="C997" s="1"/>
-      <c r="D997" s="1"/>
-      <c r="E997" s="1"/>
-      <c r="F997" s="1"/>
-      <c r="G997" s="1"/>
-      <c r="H997" s="1"/>
-      <c r="I997" s="1"/>
-      <c r="J997" s="1"/>
-      <c r="K997" s="1"/>
-      <c r="L997" s="1"/>
-      <c r="M997" s="1"/>
-      <c r="N997" s="1"/>
-      <c r="O997" s="1"/>
-      <c r="P997" s="1"/>
-      <c r="Q997" s="1"/>
-      <c r="R997" s="1"/>
-      <c r="S997" s="1"/>
-      <c r="T997" s="1"/>
-      <c r="U997" s="1"/>
-      <c r="V997" s="1"/>
-      <c r="W997" s="1"/>
-      <c r="X997" s="1"/>
-      <c r="Y997" s="1"/>
-      <c r="Z997" s="1"/>
-    </row>
-    <row r="998" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A998" s="1"/>
-      <c r="B998" s="1"/>
-      <c r="C998" s="1"/>
-      <c r="D998" s="1"/>
-      <c r="E998" s="1"/>
-      <c r="F998" s="1"/>
-      <c r="G998" s="1"/>
-      <c r="H998" s="1"/>
-      <c r="I998" s="1"/>
-      <c r="J998" s="1"/>
-      <c r="K998" s="1"/>
-      <c r="L998" s="1"/>
-      <c r="M998" s="1"/>
-      <c r="N998" s="1"/>
-      <c r="O998" s="1"/>
-      <c r="P998" s="1"/>
-      <c r="Q998" s="1"/>
-      <c r="R998" s="1"/>
-      <c r="S998" s="1"/>
-      <c r="T998" s="1"/>
-      <c r="U998" s="1"/>
-      <c r="V998" s="1"/>
-      <c r="W998" s="1"/>
-      <c r="X998" s="1"/>
-      <c r="Y998" s="1"/>
-      <c r="Z998" s="1"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E173">
-    <sortCondition ref="A2:A173"/>
-    <sortCondition ref="B2:B173"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z994">
+    <sortCondition ref="A2:A994"/>
+    <sortCondition ref="B2:B994"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101D3418-EC89-FB48-B267-17375807E4FE}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed front page + small fixes
</commit_message>
<xml_diff>
--- a/SporsmålNidarus.xlsx
+++ b/SporsmålNidarus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Documents/NTNU/Prosjekt-S22/drikkelek2022-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6920E6B-0B87-B04E-8B0D-37F431765016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3754F9E-6131-E042-9ACB-AFB199C9824A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -578,9 +578,6 @@
     <t>Hvem har høyest bodycount?</t>
   </si>
   <si>
-    <t>Personen som onanerte sist kan dele ut 2 slurker</t>
-  </si>
-  <si>
     <t>memb, gi en slurk til den med høyest standard</t>
   </si>
   <si>
@@ -600,6 +597,9 @@
   </si>
   <si>
     <t xml:space="preserve">Stirrekonkurranse mellom memb og memb2. Vinneren deler ut 6 slurker. </t>
+  </si>
+  <si>
+    <t>Personen som onanerte sist kan dele ut 4 slurker</t>
   </si>
 </sst>
 </file>
@@ -990,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266B615A-CB75-A44D-9106-24B2B9F7FAAE}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView topLeftCell="A51" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3787,7 +3787,7 @@
         <v>0</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -4183,7 +4183,7 @@
         <v>0</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>42</v>
@@ -4651,7 +4651,7 @@
         <v>1</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
@@ -6091,7 +6091,7 @@
         <v>0</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
@@ -6702,7 +6702,7 @@
         <v>1</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E159" s="2"/>
       <c r="F159" s="1"/>
@@ -6738,7 +6738,7 @@
         <v>0</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E160" s="1"/>
       <c r="F160" s="1"/>
@@ -30048,8 +30048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101D3418-EC89-FB48-B267-17375807E4FE}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30518,7 +30518,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -30571,7 +30571,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed start page headine + redesigned "legg til spillere"-button
</commit_message>
<xml_diff>
--- a/SporsmålNidarus.xlsx
+++ b/SporsmålNidarus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Documents/NTNU/Prosjekt-S22/drikkelek2022-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3754F9E-6131-E042-9ACB-AFB199C9824A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F318F898-D44F-BF47-ADFD-0559ED4C493D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="190">
   <si>
     <t>Kategori</t>
   </si>
@@ -601,6 +601,12 @@
   <si>
     <t>Personen som onanerte sist kan dele ut 4 slurker</t>
   </si>
+  <si>
+    <t>Den første som sier "ja" må chugge</t>
+  </si>
+  <si>
+    <t>memb og memb2 kan legge til utfordringer</t>
+  </si>
 </sst>
 </file>
 
@@ -990,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266B615A-CB75-A44D-9106-24B2B9F7FAAE}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6764,10 +6770,18 @@
       <c r="Z160" s="1"/>
     </row>
     <row r="161" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A161" s="2"/>
-      <c r="B161" s="1"/>
-      <c r="C161" s="2"/>
-      <c r="D161" s="2"/>
+      <c r="A161" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B161" s="3">
+        <v>1</v>
+      </c>
+      <c r="C161" s="3">
+        <v>0</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="E161" s="2"/>
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
@@ -6792,10 +6806,18 @@
       <c r="Z161" s="1"/>
     </row>
     <row r="162" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A162" s="2"/>
-      <c r="B162" s="1"/>
-      <c r="C162" s="2"/>
-      <c r="D162" s="2"/>
+      <c r="A162" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B162" s="3">
+        <v>1</v>
+      </c>
+      <c r="C162" s="3">
+        <v>0</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="E162" s="2"/>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
@@ -30046,10 +30068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101D3418-EC89-FB48-B267-17375807E4FE}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A10" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30574,6 +30596,20 @@
         <v>182</v>
       </c>
     </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated questions + small fix + changed design
</commit_message>
<xml_diff>
--- a/SporsmålNidarus.xlsx
+++ b/SporsmålNidarus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Documents/NTNU/Prosjekt-S22/drikkelek2022-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F318F898-D44F-BF47-ADFD-0559ED4C493D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEDE704-F3A1-F140-84FD-58D111C20CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="211">
   <si>
     <t>Kategori</t>
   </si>
@@ -602,10 +602,73 @@
     <t>Personen som onanerte sist kan dele ut 4 slurker</t>
   </si>
   <si>
-    <t>Den første som sier "ja" må chugge</t>
+    <t>memb og memb2 kan legge til utfordringer</t>
   </si>
   <si>
-    <t>memb og memb2 kan legge til utfordringer</t>
+    <t>Jeg har aldri hatt sex i en bil</t>
+  </si>
+  <si>
+    <t>Jeg har aldri pult på første date </t>
+  </si>
+  <si>
+    <t>Jeg har aldri svelget</t>
+  </si>
+  <si>
+    <t>Jeg har aldri pult mer enn tre ganger på en dag</t>
+  </si>
+  <si>
+    <t>Jeg har aldri onanert mer enn fire ganger på en dag</t>
+  </si>
+  <si>
+    <t>Jeg har aldri pult i en dusj</t>
+  </si>
+  <si>
+    <t>Jeg har aldri kastet opp dagen derpå</t>
+  </si>
+  <si>
+    <t>Hvem kunne du hooket? Personen med flest pek setter på sin beste hookesang. </t>
+  </si>
+  <si>
+    <t>Memb, kyss en i rommet. Personen kan dele ut 4 slurker. </t>
+  </si>
+  <si>
+    <t>Hvem passer best på et midtsidebilde</t>
+  </si>
+  <si>
+    <t>Hvem er den største playeren </t>
+  </si>
+  <si>
+    <t>Memb, hvem skal chugge med deg?</t>
+  </si>
+  <si>
+    <t>Jeg har aldri pult i skogen</t>
+  </si>
+  <si>
+    <t>Jeg har aldri pult i havet</t>
+  </si>
+  <si>
+    <t>Drikk hvis du har blitt nektet inngang på et utested</t>
+  </si>
+  <si>
+    <t>Drikk hvis du søkte indøk </t>
+  </si>
+  <si>
+    <t>Hvem ville laget den beste pornofilmen med deg?</t>
+  </si>
+  <si>
+    <t>Hvem ville tjent mest på onlyfans?</t>
+  </si>
+  <si>
+    <t>Hvem skal chugge drikken sin?</t>
+  </si>
+  <si>
+    <t>Hvem er stuck i milla?</t>
+  </si>
+  <si>
+    <t>Jeg har aldri tatt en angrepille</t>
+  </si>
+  <si>
+    <t>Den første som sier \"ja\" må chugge</t>
   </si>
 </sst>
 </file>
@@ -996,7 +1059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266B615A-CB75-A44D-9106-24B2B9F7FAAE}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="135" workbookViewId="0">
+    <sheetView topLeftCell="A152" zoomScale="135" workbookViewId="0">
       <selection activeCell="D166" sqref="D166"/>
     </sheetView>
   </sheetViews>
@@ -6780,7 +6843,7 @@
         <v>0</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E161" s="2"/>
       <c r="F161" s="1"/>
@@ -6816,7 +6879,7 @@
         <v>0</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E162" s="2"/>
       <c r="F162" s="1"/>
@@ -30068,17 +30131,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101D3418-EC89-FB48-B267-17375807E4FE}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="140" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="63.33203125" customWidth="1"/>
+    <col min="4" max="4" width="78.5" customWidth="1"/>
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -30174,7 +30237,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -30231,7 +30294,7 @@
         <v>49</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -30248,7 +30311,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -30371,7 +30434,7 @@
         <v>49</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -30388,7 +30451,7 @@
         <v>49</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -30601,13 +30664,307 @@
         <v>144</v>
       </c>
       <c r="B30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>188</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36" s="1">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="1">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="1">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated front page and added google tag
</commit_message>
<xml_diff>
--- a/SporsmålNidarus.xlsx
+++ b/SporsmålNidarus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecilia/Documents/NTNU/Prosjekt-S22/drikkelek2022-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEDE704-F3A1-F140-84FD-58D111C20CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE6F3E5-A5B5-D645-8E68-257B230912D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16120" xr2:uid="{3476C9CD-C88E-924B-8DF1-FDF23DE56CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="210">
   <si>
     <t>Kategori</t>
   </si>
@@ -539,9 +539,6 @@
     <t xml:space="preserve">memb, ta håndbak med memb2. Vinneren deler ut 4 slurker. </t>
   </si>
   <si>
-    <t>memb, hva er de 3 viktigste egenskapene du ser etter i en partner?</t>
-  </si>
-  <si>
     <t>Hvem får flest superlikes på Tinder?</t>
   </si>
   <si>
@@ -735,13 +732,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1057,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266B615A-CB75-A44D-9106-24B2B9F7FAAE}">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1072,19 +1068,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1"/>
@@ -1109,19 +1105,18 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="2"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1145,19 +1140,18 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>0</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1181,19 +1175,18 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1253,16 +1246,16 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>151</v>
       </c>
       <c r="F6" s="1"/>
@@ -1370,7 +1363,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1396,19 +1389,18 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="2"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1432,19 +1424,18 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1504,19 +1495,18 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="2"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1540,19 +1530,18 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>0</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="2"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1586,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1648,19 +1637,18 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>0</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="2"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1684,19 +1672,18 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="2"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1720,19 +1707,18 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>0</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="2"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1756,19 +1742,18 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>0</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="2"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1792,19 +1777,18 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="1">
         <v>3</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>0</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="2"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1828,19 +1812,18 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>0</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="2"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1864,19 +1847,18 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="1">
         <v>3</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="2"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1900,19 +1882,18 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1">
         <v>3</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>0</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="2"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1936,19 +1917,18 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25">
         <v>0</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
         <v>0</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="2"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1972,19 +1952,19 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26">
         <v>0</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" t="s">
         <v>32</v>
       </c>
       <c r="F26" s="1"/>
@@ -2010,19 +1990,18 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27">
         <v>0</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="2"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2046,19 +2025,18 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28">
         <v>0</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="2"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2118,19 +2096,18 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>0</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>1</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="2"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2154,19 +2131,18 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="2"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2226,19 +2202,18 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33">
         <v>0</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="2"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2262,19 +2237,18 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34">
         <v>0</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="2"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2298,19 +2272,18 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="2"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2334,19 +2307,18 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36">
         <v>1</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" t="s">
         <v>22</v>
       </c>
-      <c r="E36" s="2"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2370,19 +2342,18 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="2"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2478,19 +2449,18 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="A40" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40">
         <v>0</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="2"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -2514,19 +2484,18 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41">
         <v>1</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41">
         <v>0</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" t="s">
         <v>83</v>
       </c>
-      <c r="E41" s="2"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -2550,19 +2519,18 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="A42" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42">
         <v>1</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42">
         <v>1</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="2"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -2586,19 +2554,18 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="A43" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43">
         <v>1</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43">
         <v>1</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="2"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -2622,19 +2589,18 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="A44" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44">
         <v>1</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44">
         <v>1</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="2"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -2658,19 +2624,18 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45">
         <v>2</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45">
         <v>0</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" t="s">
         <v>92</v>
       </c>
-      <c r="E45" s="2"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -2694,19 +2659,18 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="A46" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46">
         <v>2</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46">
         <v>0</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" t="s">
         <v>39</v>
       </c>
-      <c r="E46" s="2"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -2730,19 +2694,18 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47">
         <v>2</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47">
         <v>0</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" t="s">
         <v>40</v>
       </c>
-      <c r="E47" s="2"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -2766,19 +2729,18 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="A48" t="s">
         <v>17</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48">
         <v>2</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48">
         <v>1</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="2"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -2802,19 +2764,18 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49">
         <v>2</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49">
         <v>1</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" t="s">
         <v>34</v>
       </c>
-      <c r="E49" s="2"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -2838,19 +2799,18 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="A50" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50">
         <v>2</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50">
         <v>1</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" t="s">
         <v>35</v>
       </c>
-      <c r="E50" s="2"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -2874,19 +2834,18 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="A51" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51">
         <v>2</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51">
         <v>1</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="2"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -2910,19 +2869,18 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="A52" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52">
         <v>2</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52">
         <v>1</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" t="s">
         <v>37</v>
       </c>
-      <c r="E52" s="2"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -2946,19 +2904,18 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="A53" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53">
         <v>2</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53">
         <v>1</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" t="s">
         <v>38</v>
       </c>
-      <c r="E53" s="2"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -3018,19 +2975,18 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="A55" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55">
         <v>0</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55">
         <v>0</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" t="s">
         <v>59</v>
       </c>
-      <c r="E55" s="2"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -3054,19 +3010,18 @@
       <c r="Z55" s="1"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+      <c r="A56" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56">
         <v>2</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56">
         <v>0</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" t="s">
         <v>148</v>
       </c>
-      <c r="E56" s="2"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -3090,19 +3045,18 @@
       <c r="Z56" s="1"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57">
         <v>2</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57">
         <v>0</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="2"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -3126,19 +3080,18 @@
       <c r="Z57" s="1"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58">
         <v>2</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58">
         <v>0</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" t="s">
         <v>68</v>
       </c>
-      <c r="E58" s="2"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
@@ -3162,19 +3115,18 @@
       <c r="Z58" s="1"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59">
         <v>3</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59">
         <v>0</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" t="s">
         <v>60</v>
       </c>
-      <c r="E59" s="2"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -3198,19 +3150,18 @@
       <c r="Z59" s="1"/>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
+      <c r="A60" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60">
         <v>2</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60">
         <v>0</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" t="s">
         <v>58</v>
       </c>
-      <c r="E60" s="2"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -3234,19 +3185,18 @@
       <c r="Z60" s="1"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+      <c r="A61" t="s">
         <v>57</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61">
         <v>2</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61">
         <v>0</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" t="s">
         <v>63</v>
       </c>
-      <c r="E61" s="2"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -3270,19 +3220,18 @@
       <c r="Z61" s="1"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62">
         <v>3</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62">
         <v>0</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" t="s">
         <v>64</v>
       </c>
-      <c r="E62" s="2"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -3306,19 +3255,18 @@
       <c r="Z62" s="1"/>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
+      <c r="A63" t="s">
         <v>57</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63">
         <v>3</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63">
         <v>1</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D63" t="s">
         <v>61</v>
       </c>
-      <c r="E63" s="2"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -3342,19 +3290,18 @@
       <c r="Z63" s="1"/>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
+      <c r="A64" t="s">
         <v>57</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64">
         <v>2</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64">
         <v>0</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D64" t="s">
         <v>124</v>
       </c>
-      <c r="E64" s="2"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
@@ -3378,19 +3325,18 @@
       <c r="Z64" s="1"/>
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
+      <c r="A65" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65">
         <v>1</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65">
         <v>0</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" t="s">
         <v>96</v>
       </c>
-      <c r="E65" s="2"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -3414,19 +3360,18 @@
       <c r="Z65" s="1"/>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
+      <c r="A66" t="s">
         <v>136</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66">
         <v>1</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66">
         <v>0</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D66" t="s">
         <v>96</v>
       </c>
-      <c r="E66" s="2"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -3450,19 +3395,18 @@
       <c r="Z66" s="1"/>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
+      <c r="A67" t="s">
         <v>136</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67">
         <v>1</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67">
         <v>0</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D67" t="s">
         <v>95</v>
       </c>
-      <c r="E67" s="2"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
@@ -3486,19 +3430,18 @@
       <c r="Z67" s="1"/>
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
+      <c r="A68" t="s">
         <v>136</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68">
         <v>1</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68">
         <v>0</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" t="s">
         <v>95</v>
       </c>
-      <c r="E68" s="2"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
@@ -3522,19 +3465,18 @@
       <c r="Z68" s="1"/>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
+      <c r="A69" t="s">
         <v>136</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69">
         <v>1</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69">
         <v>0</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D69" t="s">
         <v>97</v>
       </c>
-      <c r="E69" s="2"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -3558,19 +3500,18 @@
       <c r="Z69" s="1"/>
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
+      <c r="A70" t="s">
         <v>136</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70">
         <v>1</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70">
         <v>0</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" t="s">
         <v>97</v>
       </c>
-      <c r="E70" s="2"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -3594,19 +3535,18 @@
       <c r="Z70" s="1"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
+      <c r="A71" t="s">
         <v>136</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71">
         <v>1</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71">
         <v>0</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" t="s">
         <v>94</v>
       </c>
-      <c r="E71" s="2"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
@@ -3630,19 +3570,18 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
+      <c r="A72" t="s">
         <v>136</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72">
         <v>1</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72">
         <v>0</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" t="s">
         <v>94</v>
       </c>
-      <c r="E72" s="2"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
@@ -3666,19 +3605,18 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
+      <c r="A73" t="s">
         <v>136</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73">
         <v>1</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73">
         <v>0</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" t="s">
         <v>95</v>
       </c>
-      <c r="E73" s="2"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
@@ -3702,19 +3640,18 @@
       <c r="Z73" s="1"/>
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
+      <c r="A74" t="s">
         <v>136</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74">
         <v>1</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74">
         <v>0</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" t="s">
         <v>95</v>
       </c>
-      <c r="E74" s="2"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
@@ -3738,19 +3675,18 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
+      <c r="A75" t="s">
         <v>41</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75">
         <v>0</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75">
         <v>0</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D75" t="s">
         <v>72</v>
       </c>
-      <c r="E75" s="2"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
@@ -3774,19 +3710,18 @@
       <c r="Z75" s="1"/>
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
+      <c r="A76" t="s">
         <v>41</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76">
         <v>0</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76">
         <v>0</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D76" t="s">
         <v>88</v>
       </c>
-      <c r="E76" s="2"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
@@ -3817,10 +3752,10 @@
         <v>0</v>
       </c>
       <c r="C77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -3846,19 +3781,18 @@
       <c r="Z77" s="1"/>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+      <c r="A78" t="s">
         <v>41</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78">
         <v>0</v>
       </c>
-      <c r="C78" s="1">
+      <c r="C78">
         <v>0</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E78" s="1"/>
+      <c r="D78" t="s">
+        <v>71</v>
+      </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
@@ -3882,19 +3816,19 @@
       <c r="Z78" s="1"/>
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
+      <c r="A79" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79">
         <v>0</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79">
         <v>0</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E79" s="2"/>
+      <c r="D79" t="s">
+        <v>149</v>
+      </c>
+      <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
@@ -3918,17 +3852,17 @@
       <c r="Z79" s="1"/>
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>0</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="1">
         <v>0</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>149</v>
+      <c r="D80" s="1" t="s">
+        <v>143</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -3954,19 +3888,18 @@
       <c r="Z80" s="1"/>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
+      <c r="A81" t="s">
         <v>41</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
         <v>0</v>
       </c>
-      <c r="C81" s="1">
-        <v>0</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E81" s="1"/>
+      <c r="D81" t="s">
+        <v>69</v>
+      </c>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
@@ -3990,19 +3923,18 @@
       <c r="Z81" s="1"/>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
+      <c r="A82" t="s">
         <v>41</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82">
         <v>1</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82">
         <v>0</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E82" s="2"/>
+      <c r="D82" t="s">
+        <v>70</v>
+      </c>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
@@ -4026,19 +3958,18 @@
       <c r="Z82" s="1"/>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A83" s="2" t="s">
+      <c r="A83" t="s">
         <v>41</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83">
         <v>1</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83">
         <v>0</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E83" s="2"/>
+      <c r="D83" t="s">
+        <v>73</v>
+      </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
@@ -4062,19 +3993,18 @@
       <c r="Z83" s="1"/>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
+      <c r="A84" t="s">
         <v>41</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84">
         <v>1</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84">
         <v>0</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E84" s="2"/>
+      <c r="D84" t="s">
+        <v>89</v>
+      </c>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
@@ -4097,20 +4027,20 @@
       <c r="Y84" s="1"/>
       <c r="Z84" s="1"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
+    <row r="85" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>41</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85">
         <v>1</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85">
         <v>0</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E85" s="2"/>
+      <c r="D85" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
@@ -4133,18 +4063,18 @@
       <c r="Y85" s="1"/>
       <c r="Z85" s="1"/>
     </row>
-    <row r="86" spans="1:26" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="1">
         <v>1</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="1">
         <v>0</v>
       </c>
-      <c r="D86" s="4" t="s">
-        <v>126</v>
+      <c r="D86" t="s">
+        <v>70</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -4179,8 +4109,8 @@
       <c r="C87" s="1">
         <v>0</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>70</v>
+      <c r="D87" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -4206,19 +4136,21 @@
       <c r="Z87" s="1"/>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>41</v>
       </c>
       <c r="B88" s="1">
         <v>1</v>
       </c>
-      <c r="C88" s="1">
+      <c r="C88">
         <v>0</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E88" s="1"/>
+      <c r="D88" t="s">
+        <v>185</v>
+      </c>
+      <c r="E88" t="s">
+        <v>42</v>
+      </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
@@ -4242,21 +4174,19 @@
       <c r="Z88" s="1"/>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B89" s="1">
         <v>1</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="1">
         <v>0</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="D89" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
@@ -4279,7 +4209,7 @@
       <c r="Y89" s="1"/>
       <c r="Z89" s="1"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>41</v>
       </c>
@@ -4289,10 +4219,9 @@
       <c r="C90" s="1">
         <v>0</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D90" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
@@ -4325,7 +4254,7 @@
       <c r="C91" s="1">
         <v>0</v>
       </c>
-      <c r="D91" s="4" t="s">
+      <c r="D91" s="3" t="s">
         <v>128</v>
       </c>
       <c r="F91" s="1"/>
@@ -4350,7 +4279,7 @@
       <c r="Y91" s="1"/>
       <c r="Z91" s="1"/>
     </row>
-    <row r="92" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>41</v>
       </c>
@@ -4360,9 +4289,10 @@
       <c r="C92" s="1">
         <v>0</v>
       </c>
-      <c r="D92" s="4" t="s">
-        <v>128</v>
-      </c>
+      <c r="D92" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
@@ -4396,7 +4326,7 @@
         <v>0</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -4422,17 +4352,17 @@
       <c r="Z93" s="1"/>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
+      <c r="A94" t="s">
         <v>41</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94">
         <v>1</v>
       </c>
-      <c r="C94" s="1">
+      <c r="C94">
         <v>0</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>140</v>
+      <c r="D94" t="s">
+        <v>70</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
@@ -4458,16 +4388,16 @@
       <c r="Z94" s="1"/>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
+      <c r="A95" t="s">
         <v>41</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95">
         <v>1</v>
       </c>
-      <c r="C95" s="2">
+      <c r="C95">
         <v>0</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D95" t="s">
         <v>70</v>
       </c>
       <c r="E95" s="1"/>
@@ -4494,17 +4424,17 @@
       <c r="Z95" s="1"/>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="1">
         <v>1</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C96" s="1">
         <v>0</v>
       </c>
-      <c r="D96" s="2" t="s">
-        <v>70</v>
+      <c r="D96" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -4540,7 +4470,7 @@
         <v>0</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -4576,7 +4506,7 @@
         <v>0</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -4609,10 +4539,10 @@
         <v>1</v>
       </c>
       <c r="C99" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -4645,10 +4575,10 @@
         <v>1</v>
       </c>
       <c r="C100" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
@@ -4684,7 +4614,7 @@
         <v>1</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
@@ -4720,7 +4650,7 @@
         <v>1</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
@@ -4750,13 +4680,13 @@
         <v>41</v>
       </c>
       <c r="B103" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C103" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
@@ -4900,7 +4830,7 @@
         <v>0</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
@@ -4936,7 +4866,7 @@
         <v>0</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>166</v>
+        <v>122</v>
       </c>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
@@ -4972,7 +4902,7 @@
         <v>0</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
@@ -5008,7 +4938,7 @@
         <v>0</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
@@ -5034,19 +4964,18 @@
       <c r="Z110" s="1"/>
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A111" s="1" t="s">
-        <v>41</v>
+      <c r="A111" t="s">
+        <v>144</v>
       </c>
       <c r="B111" s="1">
         <v>2</v>
       </c>
-      <c r="C111" s="1">
+      <c r="C111">
         <v>0</v>
       </c>
-      <c r="D111" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E111" s="1"/>
+      <c r="D111" t="s">
+        <v>84</v>
+      </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
@@ -5070,19 +4999,18 @@
       <c r="Z111" s="1"/>
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
+      <c r="A112" t="s">
         <v>41</v>
       </c>
       <c r="B112" s="1">
         <v>2</v>
       </c>
-      <c r="C112" s="2">
+      <c r="C112">
         <v>0</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E112" s="2"/>
+      <c r="D112" t="s">
+        <v>74</v>
+      </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
@@ -5106,19 +5034,18 @@
       <c r="Z112" s="1"/>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
+      <c r="A113" t="s">
         <v>41</v>
       </c>
       <c r="B113" s="1">
         <v>2</v>
       </c>
-      <c r="C113" s="2">
+      <c r="C113">
         <v>0</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E113" s="2"/>
+      <c r="D113" t="s">
+        <v>75</v>
+      </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
@@ -5142,19 +5069,18 @@
       <c r="Z113" s="1"/>
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
+      <c r="A114" t="s">
         <v>41</v>
       </c>
       <c r="B114" s="1">
-        <v>2</v>
-      </c>
-      <c r="C114" s="2">
+        <v>3</v>
+      </c>
+      <c r="C114">
         <v>0</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E114" s="2"/>
+      <c r="D114" t="s">
+        <v>87</v>
+      </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
@@ -5178,19 +5104,18 @@
       <c r="Z114" s="1"/>
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A115" s="2" t="s">
+      <c r="A115" t="s">
         <v>41</v>
       </c>
       <c r="B115" s="1">
-        <v>3</v>
-      </c>
-      <c r="C115" s="2">
+        <v>2</v>
+      </c>
+      <c r="C115">
         <v>0</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E115" s="2"/>
+      <c r="D115" t="s">
+        <v>76</v>
+      </c>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
@@ -5214,19 +5139,19 @@
       <c r="Z115" s="1"/>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A116" s="2" t="s">
+      <c r="A116" t="s">
         <v>41</v>
       </c>
       <c r="B116" s="1">
         <v>2</v>
       </c>
-      <c r="C116" s="2">
+      <c r="C116">
         <v>0</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E116" s="2"/>
+      <c r="D116" t="s">
+        <v>99</v>
+      </c>
+      <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
@@ -5250,17 +5175,17 @@
       <c r="Z116" s="1"/>
     </row>
     <row r="117" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B117" s="1">
         <v>2</v>
       </c>
-      <c r="C117" s="2">
+      <c r="C117" s="1">
         <v>0</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>99</v>
+      <c r="D117" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
@@ -5286,19 +5211,18 @@
       <c r="Z117" s="1"/>
     </row>
     <row r="118" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A118" s="1" t="s">
+      <c r="A118" t="s">
         <v>41</v>
       </c>
       <c r="B118" s="1">
         <v>2</v>
       </c>
-      <c r="C118" s="1">
+      <c r="C118">
         <v>0</v>
       </c>
-      <c r="D118" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E118" s="1"/>
+      <c r="D118" t="s">
+        <v>78</v>
+      </c>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
@@ -5322,19 +5246,18 @@
       <c r="Z118" s="1"/>
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A119" s="2" t="s">
+      <c r="A119" t="s">
         <v>41</v>
       </c>
       <c r="B119" s="1">
         <v>2</v>
       </c>
-      <c r="C119" s="2">
+      <c r="C119">
         <v>0</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E119" s="2"/>
+      <c r="D119" t="s">
+        <v>90</v>
+      </c>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
@@ -5358,19 +5281,19 @@
       <c r="Z119" s="1"/>
     </row>
     <row r="120" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B120" s="1">
         <v>2</v>
       </c>
-      <c r="C120" s="2">
+      <c r="C120" s="1">
         <v>0</v>
       </c>
-      <c r="D120" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E120" s="2"/>
+      <c r="D120" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E120" s="1"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
@@ -5404,7 +5327,7 @@
         <v>0</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
@@ -5430,19 +5353,18 @@
       <c r="Z121" s="1"/>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
+      <c r="A122" t="s">
         <v>41</v>
       </c>
       <c r="B122" s="1">
         <v>2</v>
       </c>
-      <c r="C122" s="1">
+      <c r="C122">
         <v>0</v>
       </c>
-      <c r="D122" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E122" s="1"/>
+      <c r="D122" t="s">
+        <v>79</v>
+      </c>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
@@ -5466,19 +5388,18 @@
       <c r="Z122" s="1"/>
     </row>
     <row r="123" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A123" s="2" t="s">
+      <c r="A123" t="s">
         <v>41</v>
       </c>
       <c r="B123" s="1">
         <v>2</v>
       </c>
-      <c r="C123" s="2">
+      <c r="C123">
         <v>0</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E123" s="2"/>
+      <c r="D123" t="s">
+        <v>85</v>
+      </c>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
@@ -5502,19 +5423,18 @@
       <c r="Z123" s="1"/>
     </row>
     <row r="124" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A124" s="2" t="s">
+      <c r="A124" t="s">
         <v>41</v>
       </c>
       <c r="B124" s="1">
         <v>2</v>
       </c>
-      <c r="C124" s="2">
-        <v>0</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E124" s="2"/>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="D124" t="s">
+        <v>129</v>
+      </c>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
@@ -5538,19 +5458,18 @@
       <c r="Z124" s="1"/>
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="s">
+      <c r="A125" t="s">
         <v>41</v>
       </c>
       <c r="B125" s="1">
         <v>2</v>
       </c>
-      <c r="C125" s="2">
-        <v>1</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E125" s="2"/>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125" t="s">
+        <v>130</v>
+      </c>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
@@ -5574,19 +5493,19 @@
       <c r="Z125" s="1"/>
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A126" s="2" t="s">
+      <c r="A126" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B126" s="1">
         <v>2</v>
       </c>
-      <c r="C126" s="2">
+      <c r="C126" s="1">
         <v>0</v>
       </c>
-      <c r="D126" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E126" s="2"/>
+      <c r="D126" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E126" s="1"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
@@ -5620,7 +5539,7 @@
         <v>0</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -5646,19 +5565,18 @@
       <c r="Z127" s="1"/>
     </row>
     <row r="128" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A128" s="1" t="s">
+      <c r="A128" t="s">
         <v>41</v>
       </c>
       <c r="B128" s="1">
         <v>2</v>
       </c>
-      <c r="C128" s="1">
+      <c r="C128">
         <v>0</v>
       </c>
-      <c r="D128" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E128" s="1"/>
+      <c r="D128" t="s">
+        <v>86</v>
+      </c>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
@@ -5682,19 +5600,19 @@
       <c r="Z128" s="1"/>
     </row>
     <row r="129" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B129" s="1">
         <v>2</v>
       </c>
-      <c r="C129" s="2">
+      <c r="C129">
         <v>0</v>
       </c>
-      <c r="D129" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E129" s="2"/>
+      <c r="D129" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
@@ -5724,11 +5642,11 @@
       <c r="B130" s="1">
         <v>2</v>
       </c>
-      <c r="C130" s="2">
+      <c r="C130" s="1">
         <v>0</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -5764,7 +5682,7 @@
         <v>0</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
@@ -5790,19 +5708,18 @@
       <c r="Z131" s="1"/>
     </row>
     <row r="132" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A132" s="1" t="s">
+      <c r="A132" t="s">
         <v>41</v>
       </c>
       <c r="B132" s="1">
-        <v>2</v>
-      </c>
-      <c r="C132" s="1">
+        <v>3</v>
+      </c>
+      <c r="C132">
         <v>0</v>
       </c>
-      <c r="D132" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E132" s="1"/>
+      <c r="D132" t="s">
+        <v>125</v>
+      </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
@@ -5826,19 +5743,19 @@
       <c r="Z132" s="1"/>
     </row>
     <row r="133" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A133" s="2" t="s">
+      <c r="A133" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B133" s="1">
         <v>3</v>
       </c>
-      <c r="C133" s="2">
+      <c r="C133" s="1">
         <v>0</v>
       </c>
-      <c r="D133" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E133" s="2"/>
+      <c r="D133" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
@@ -5862,19 +5779,18 @@
       <c r="Z133" s="1"/>
     </row>
     <row r="134" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A134" s="1" t="s">
+      <c r="A134" t="s">
         <v>41</v>
       </c>
       <c r="B134" s="1">
         <v>3</v>
       </c>
-      <c r="C134" s="1">
+      <c r="C134">
         <v>0</v>
       </c>
-      <c r="D134" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E134" s="1"/>
+      <c r="D134" t="s">
+        <v>98</v>
+      </c>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
@@ -5898,19 +5814,18 @@
       <c r="Z134" s="1"/>
     </row>
     <row r="135" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A135" s="2" t="s">
+      <c r="A135" t="s">
         <v>41</v>
       </c>
       <c r="B135" s="1">
         <v>3</v>
       </c>
-      <c r="C135" s="2">
+      <c r="C135">
         <v>0</v>
       </c>
-      <c r="D135" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E135" s="2"/>
+      <c r="D135" t="s">
+        <v>77</v>
+      </c>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
@@ -5934,19 +5849,18 @@
       <c r="Z135" s="1"/>
     </row>
     <row r="136" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A136" s="2" t="s">
+      <c r="A136" t="s">
         <v>41</v>
       </c>
       <c r="B136" s="1">
         <v>3</v>
       </c>
-      <c r="C136" s="2">
+      <c r="C136">
         <v>0</v>
       </c>
-      <c r="D136" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E136" s="2"/>
+      <c r="D136" t="s">
+        <v>134</v>
+      </c>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
@@ -5970,19 +5884,18 @@
       <c r="Z136" s="1"/>
     </row>
     <row r="137" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A137" s="2" t="s">
+      <c r="A137" t="s">
         <v>41</v>
       </c>
       <c r="B137" s="1">
         <v>3</v>
       </c>
-      <c r="C137" s="2">
+      <c r="C137">
         <v>0</v>
       </c>
-      <c r="D137" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E137" s="2"/>
+      <c r="D137" t="s">
+        <v>80</v>
+      </c>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
@@ -6006,19 +5919,19 @@
       <c r="Z137" s="1"/>
     </row>
     <row r="138" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A138" s="2" t="s">
+      <c r="A138" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B138" s="1">
         <v>3</v>
       </c>
-      <c r="C138" s="2">
+      <c r="C138" s="1">
         <v>0</v>
       </c>
-      <c r="D138" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E138" s="2"/>
+      <c r="D138" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E138" s="1"/>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
@@ -6052,7 +5965,7 @@
         <v>0</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
@@ -6088,7 +6001,7 @@
         <v>0</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
@@ -6124,7 +6037,7 @@
         <v>0</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
@@ -6160,7 +6073,7 @@
         <v>0</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
@@ -6196,7 +6109,7 @@
         <v>0</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
@@ -6222,19 +6135,18 @@
       <c r="Z143" s="1"/>
     </row>
     <row r="144" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A144" s="1" t="s">
-        <v>41</v>
+      <c r="A144" t="s">
+        <v>100</v>
       </c>
       <c r="B144" s="1">
-        <v>3</v>
-      </c>
-      <c r="C144" s="1">
         <v>0</v>
       </c>
-      <c r="D144" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E144" s="1"/>
+      <c r="C144">
+        <v>1</v>
+      </c>
+      <c r="D144" t="s">
+        <v>43</v>
+      </c>
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
@@ -6258,19 +6170,18 @@
       <c r="Z144" s="1"/>
     </row>
     <row r="145" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A145" s="2" t="s">
+      <c r="A145" t="s">
         <v>100</v>
       </c>
       <c r="B145" s="1">
         <v>0</v>
       </c>
-      <c r="C145" s="2">
+      <c r="C145">
         <v>1</v>
       </c>
-      <c r="D145" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E145" s="2"/>
+      <c r="D145" t="s">
+        <v>44</v>
+      </c>
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
@@ -6294,19 +6205,18 @@
       <c r="Z145" s="1"/>
     </row>
     <row r="146" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A146" s="2" t="s">
+      <c r="A146" t="s">
         <v>100</v>
       </c>
       <c r="B146" s="1">
         <v>0</v>
       </c>
-      <c r="C146" s="2">
+      <c r="C146">
         <v>1</v>
       </c>
-      <c r="D146" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E146" s="2"/>
+      <c r="D146" t="s">
+        <v>45</v>
+      </c>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
@@ -6330,19 +6240,18 @@
       <c r="Z146" s="1"/>
     </row>
     <row r="147" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A147" s="2" t="s">
+      <c r="A147" t="s">
         <v>100</v>
       </c>
       <c r="B147" s="1">
         <v>0</v>
       </c>
-      <c r="C147" s="2">
+      <c r="C147">
         <v>1</v>
       </c>
-      <c r="D147" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E147" s="2"/>
+      <c r="D147" t="s">
+        <v>46</v>
+      </c>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
@@ -6366,19 +6275,19 @@
       <c r="Z147" s="1"/>
     </row>
     <row r="148" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A148" s="2" t="s">
+      <c r="A148" t="s">
         <v>100</v>
       </c>
       <c r="B148" s="1">
         <v>0</v>
       </c>
-      <c r="C148" s="2">
+      <c r="C148" s="1">
         <v>1</v>
       </c>
-      <c r="D148" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E148" s="2"/>
+      <c r="D148" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E148" s="1"/>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
@@ -6402,17 +6311,17 @@
       <c r="Z148" s="1"/>
     </row>
     <row r="149" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A149" s="2" t="s">
+      <c r="A149" t="s">
         <v>100</v>
       </c>
       <c r="B149" s="1">
         <v>0</v>
       </c>
-      <c r="C149" s="1">
+      <c r="C149">
         <v>1</v>
       </c>
-      <c r="D149" s="1" t="s">
-        <v>107</v>
+      <c r="D149" t="s">
+        <v>101</v>
       </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
@@ -6438,19 +6347,18 @@
       <c r="Z149" s="1"/>
     </row>
     <row r="150" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A150" s="2" t="s">
+      <c r="A150" t="s">
         <v>100</v>
       </c>
       <c r="B150" s="1">
         <v>0</v>
       </c>
-      <c r="C150" s="2">
-        <v>1</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E150" s="1"/>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150" t="s">
+        <v>137</v>
+      </c>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
@@ -6474,17 +6382,17 @@
       <c r="Z150" s="1"/>
     </row>
     <row r="151" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A151" s="2" t="s">
+      <c r="A151" t="s">
         <v>100</v>
       </c>
       <c r="B151" s="1">
         <v>0</v>
       </c>
-      <c r="C151" s="2">
-        <v>0</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>137</v>
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="D151" t="s">
+        <v>47</v>
       </c>
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
@@ -6509,19 +6417,18 @@
       <c r="Z151" s="1"/>
     </row>
     <row r="152" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A152" s="2" t="s">
+      <c r="A152" t="s">
         <v>100</v>
       </c>
       <c r="B152" s="1">
-        <v>0</v>
-      </c>
-      <c r="C152" s="2">
         <v>1</v>
       </c>
-      <c r="D152" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E152" s="2"/>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152" t="s">
+        <v>48</v>
+      </c>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
@@ -6545,19 +6452,19 @@
       <c r="Z152" s="1"/>
     </row>
     <row r="153" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A153" s="2" t="s">
-        <v>100</v>
+      <c r="A153" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B153" s="1">
-        <v>1</v>
-      </c>
-      <c r="C153" s="2">
-        <v>1</v>
-      </c>
-      <c r="D153" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E153" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="C153" s="1">
+        <v>0</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E153" s="1"/>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
@@ -6591,7 +6498,7 @@
         <v>0</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
@@ -6617,17 +6524,17 @@
       <c r="Z154" s="1"/>
     </row>
     <row r="155" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A155" s="1" t="s">
+      <c r="A155" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B155" s="1">
+      <c r="B155" s="5">
         <v>0</v>
       </c>
-      <c r="C155" s="1">
+      <c r="C155" s="5">
         <v>0</v>
       </c>
-      <c r="D155" s="1" t="s">
-        <v>104</v>
+      <c r="D155" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
@@ -6653,17 +6560,17 @@
       <c r="Z155" s="1"/>
     </row>
     <row r="156" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A156" s="6" t="s">
+      <c r="A156" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B156" s="6">
+      <c r="B156" s="1">
         <v>0</v>
       </c>
-      <c r="C156" s="6">
+      <c r="C156" s="1">
         <v>0</v>
       </c>
-      <c r="D156" s="6" t="s">
-        <v>146</v>
+      <c r="D156" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
@@ -6699,7 +6606,7 @@
         <v>0</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
@@ -6726,18 +6633,17 @@
     </row>
     <row r="158" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="B158" s="1">
         <v>0</v>
       </c>
       <c r="C158" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E158" s="1"/>
+        <v>182</v>
+      </c>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
@@ -6762,18 +6668,18 @@
     </row>
     <row r="159" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="B159" s="1">
+        <v>2</v>
+      </c>
+      <c r="C159" s="1">
         <v>0</v>
-      </c>
-      <c r="C159" s="1">
-        <v>1</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E159" s="2"/>
+      <c r="E159" s="1"/>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
@@ -6797,19 +6703,18 @@
       <c r="Z159" s="1"/>
     </row>
     <row r="160" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A160" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B160" s="1">
-        <v>2</v>
-      </c>
-      <c r="C160" s="1">
+      <c r="A160" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B160" s="2">
+        <v>1</v>
+      </c>
+      <c r="C160" s="2">
         <v>0</v>
       </c>
-      <c r="D160" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E160" s="1"/>
+      <c r="D160" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
@@ -6833,19 +6738,18 @@
       <c r="Z160" s="1"/>
     </row>
     <row r="161" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A161" s="3" t="s">
+      <c r="A161" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B161" s="3">
+      <c r="B161" s="2">
         <v>1</v>
       </c>
-      <c r="C161" s="3">
+      <c r="C161" s="2">
         <v>0</v>
       </c>
-      <c r="D161" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E161" s="2"/>
+      <c r="D161" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
@@ -6869,19 +6773,7 @@
       <c r="Z161" s="1"/>
     </row>
     <row r="162" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A162" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B162" s="3">
-        <v>1</v>
-      </c>
-      <c r="C162" s="3">
-        <v>0</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E162" s="2"/>
+      <c r="B162" s="1"/>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
@@ -6905,11 +6797,11 @@
       <c r="Z162" s="1"/>
     </row>
     <row r="163" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A163" s="2"/>
+      <c r="A163" s="1"/>
       <c r="B163" s="1"/>
-      <c r="C163" s="2"/>
-      <c r="D163" s="2"/>
-      <c r="E163" s="2"/>
+      <c r="C163" s="1"/>
+      <c r="D163" s="1"/>
+      <c r="E163" s="1"/>
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
@@ -6961,11 +6853,7 @@
       <c r="Z164" s="1"/>
     </row>
     <row r="165" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A165" s="1"/>
       <c r="B165" s="1"/>
-      <c r="C165" s="1"/>
-      <c r="D165" s="1"/>
-      <c r="E165" s="1"/>
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
@@ -6989,11 +6877,7 @@
       <c r="Z165" s="1"/>
     </row>
     <row r="166" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A166" s="2"/>
       <c r="B166" s="1"/>
-      <c r="C166" s="2"/>
-      <c r="D166" s="2"/>
-      <c r="E166" s="2"/>
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
@@ -7017,11 +6901,11 @@
       <c r="Z166" s="1"/>
     </row>
     <row r="167" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A167" s="2"/>
+      <c r="A167" s="1"/>
       <c r="B167" s="1"/>
-      <c r="C167" s="2"/>
-      <c r="D167" s="2"/>
-      <c r="E167" s="2"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
@@ -7075,7 +6959,6 @@
     <row r="169" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
-      <c r="C169" s="1"/>
       <c r="D169" s="1"/>
       <c r="E169" s="1"/>
       <c r="F169" s="1"/>
@@ -7103,6 +6986,7 @@
     <row r="170" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
@@ -7212,11 +7096,7 @@
       <c r="Z173" s="1"/>
     </row>
     <row r="174" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A174" s="1"/>
       <c r="B174" s="1"/>
-      <c r="C174" s="1"/>
-      <c r="D174" s="1"/>
-      <c r="E174" s="1"/>
       <c r="F174" s="1"/>
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
@@ -7240,11 +7120,7 @@
       <c r="Z174" s="1"/>
     </row>
     <row r="175" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A175" s="2"/>
       <c r="B175" s="1"/>
-      <c r="C175" s="2"/>
-      <c r="D175" s="2"/>
-      <c r="E175" s="2"/>
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
@@ -7268,11 +7144,7 @@
       <c r="Z175" s="1"/>
     </row>
     <row r="176" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A176" s="2"/>
       <c r="B176" s="1"/>
-      <c r="C176" s="2"/>
-      <c r="D176" s="2"/>
-      <c r="E176" s="2"/>
       <c r="F176" s="1"/>
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
@@ -7296,11 +7168,7 @@
       <c r="Z176" s="1"/>
     </row>
     <row r="177" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A177" s="2"/>
       <c r="B177" s="1"/>
-      <c r="C177" s="2"/>
-      <c r="D177" s="2"/>
-      <c r="E177" s="2"/>
       <c r="F177" s="1"/>
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
@@ -7324,11 +7192,7 @@
       <c r="Z177" s="1"/>
     </row>
     <row r="178" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A178" s="2"/>
       <c r="B178" s="1"/>
-      <c r="C178" s="2"/>
-      <c r="D178" s="2"/>
-      <c r="E178" s="2"/>
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
@@ -7352,11 +7216,11 @@
       <c r="Z178" s="1"/>
     </row>
     <row r="179" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A179" s="2"/>
+      <c r="A179" s="1"/>
       <c r="B179" s="1"/>
-      <c r="C179" s="2"/>
-      <c r="D179" s="2"/>
-      <c r="E179" s="2"/>
+      <c r="C179" s="1"/>
+      <c r="D179" s="1"/>
+      <c r="E179" s="1"/>
       <c r="F179" s="1"/>
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
@@ -7408,11 +7272,7 @@
       <c r="Z180" s="1"/>
     </row>
     <row r="181" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A181" s="1"/>
       <c r="B181" s="1"/>
-      <c r="C181" s="1"/>
-      <c r="D181" s="1"/>
-      <c r="E181" s="1"/>
       <c r="F181" s="1"/>
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
@@ -7436,11 +7296,11 @@
       <c r="Z181" s="1"/>
     </row>
     <row r="182" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A182" s="2"/>
+      <c r="A182" s="1"/>
       <c r="B182" s="1"/>
-      <c r="C182" s="2"/>
-      <c r="D182" s="2"/>
-      <c r="E182" s="2"/>
+      <c r="C182" s="1"/>
+      <c r="D182" s="1"/>
+      <c r="E182" s="1"/>
       <c r="F182" s="1"/>
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
@@ -7467,7 +7327,6 @@
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
-      <c r="D183" s="1"/>
       <c r="E183" s="1"/>
       <c r="F183" s="1"/>
       <c r="G183" s="1"/>
@@ -7522,6 +7381,7 @@
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
+      <c r="D185" s="1"/>
       <c r="E185" s="1"/>
       <c r="F185" s="1"/>
       <c r="G185" s="1"/>
@@ -7574,18 +7434,6 @@
       <c r="Z186" s="1"/>
     </row>
     <row r="187" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A187" s="1"/>
-      <c r="B187" s="1"/>
-      <c r="C187" s="1"/>
-      <c r="D187" s="1"/>
-      <c r="E187" s="1"/>
-      <c r="F187" s="1"/>
-      <c r="G187" s="1"/>
-      <c r="H187" s="1"/>
-      <c r="I187" s="1"/>
-      <c r="J187" s="1"/>
-      <c r="K187" s="1"/>
-      <c r="L187" s="1"/>
       <c r="M187" s="1"/>
       <c r="N187" s="1"/>
       <c r="O187" s="1"/>
@@ -7602,6 +7450,18 @@
       <c r="Z187" s="1"/>
     </row>
     <row r="188" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A188" s="1"/>
+      <c r="B188" s="1"/>
+      <c r="C188" s="1"/>
+      <c r="D188" s="1"/>
+      <c r="E188" s="1"/>
+      <c r="F188" s="1"/>
+      <c r="G188" s="1"/>
+      <c r="H188" s="1"/>
+      <c r="I188" s="1"/>
+      <c r="J188" s="1"/>
+      <c r="K188" s="1"/>
+      <c r="L188" s="1"/>
       <c r="M188" s="1"/>
       <c r="N188" s="1"/>
       <c r="O188" s="1"/>
@@ -11230,11 +11090,6 @@
       <c r="Z317" s="1"/>
     </row>
     <row r="318" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A318" s="1"/>
-      <c r="B318" s="1"/>
-      <c r="C318" s="1"/>
-      <c r="D318" s="1"/>
-      <c r="E318" s="1"/>
       <c r="F318" s="1"/>
       <c r="G318" s="1"/>
       <c r="H318" s="1"/>
@@ -11281,6 +11136,11 @@
       <c r="Z319" s="1"/>
     </row>
     <row r="320" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A320" s="1"/>
+      <c r="B320" s="1"/>
+      <c r="C320" s="1"/>
+      <c r="D320" s="1"/>
+      <c r="E320" s="1"/>
       <c r="F320" s="1"/>
       <c r="G320" s="1"/>
       <c r="H320" s="1"/>
@@ -30091,38 +29951,10 @@
       <c r="Y991" s="1"/>
       <c r="Z991" s="1"/>
     </row>
-    <row r="992" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A992" s="1"/>
-      <c r="B992" s="1"/>
-      <c r="C992" s="1"/>
-      <c r="D992" s="1"/>
-      <c r="E992" s="1"/>
-      <c r="F992" s="1"/>
-      <c r="G992" s="1"/>
-      <c r="H992" s="1"/>
-      <c r="I992" s="1"/>
-      <c r="J992" s="1"/>
-      <c r="K992" s="1"/>
-      <c r="L992" s="1"/>
-      <c r="M992" s="1"/>
-      <c r="N992" s="1"/>
-      <c r="O992" s="1"/>
-      <c r="P992" s="1"/>
-      <c r="Q992" s="1"/>
-      <c r="R992" s="1"/>
-      <c r="S992" s="1"/>
-      <c r="T992" s="1"/>
-      <c r="U992" s="1"/>
-      <c r="V992" s="1"/>
-      <c r="W992" s="1"/>
-      <c r="X992" s="1"/>
-      <c r="Y992" s="1"/>
-      <c r="Z992" s="1"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z992">
-    <sortCondition ref="A2:A992"/>
-    <sortCondition ref="B2:B992"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z991">
+    <sortCondition ref="A2:A991"/>
+    <sortCondition ref="B2:B991"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30133,7 +29965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101D3418-EC89-FB48-B267-17375807E4FE}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="140" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="140" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -30146,36 +29978,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>56</v>
       </c>
       <c r="F2" s="1"/>
@@ -30199,16 +30031,16 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>162</v>
       </c>
       <c r="E4" s="1"/>
@@ -30226,64 +30058,64 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>56</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>56</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>49</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" t="s">
         <v>56</v>
       </c>
       <c r="F8" s="1"/>
@@ -30324,38 +30156,38 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>49</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>0</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>150</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" t="s">
         <v>56</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" t="s">
         <v>56</v>
       </c>
       <c r="F12" s="1"/>
@@ -30423,7 +30255,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -30457,7 +30289,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -30481,95 +30313,95 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="1">
         <v>2</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>0</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" t="s">
         <v>56</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>49</v>
       </c>
       <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" t="s">
         <v>56</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="1">
         <v>2</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="D22" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" t="s">
         <v>56</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>0</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" t="s">
         <v>54</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" t="s">
         <v>56</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>49</v>
       </c>
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>0</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" t="s">
         <v>56</v>
       </c>
       <c r="F24" s="1"/>
@@ -30603,26 +30435,26 @@
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="1">
         <v>3</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" t="s">
         <v>132</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" t="s">
         <v>81</v>
       </c>
       <c r="F27" s="1"/>
@@ -30656,7 +30488,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -30670,7 +30502,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -30683,8 +30515,8 @@
       <c r="C31" s="1">
         <v>0</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>208</v>
+      <c r="D31" s="3" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -30697,8 +30529,8 @@
       <c r="C32" s="1">
         <v>0</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>189</v>
+      <c r="D32" s="3" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30711,8 +30543,8 @@
       <c r="C33" s="1">
         <v>0</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>190</v>
+      <c r="D33" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30725,8 +30557,8 @@
       <c r="C34" s="1">
         <v>0</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>209</v>
+      <c r="D34" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30739,8 +30571,8 @@
       <c r="C35" s="1">
         <v>0</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>191</v>
+      <c r="D35" s="3" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30753,8 +30585,8 @@
       <c r="C36" s="1">
         <v>0</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>192</v>
+      <c r="D36" s="3" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30767,8 +30599,8 @@
       <c r="C37" s="1">
         <v>0</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>193</v>
+      <c r="D37" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30781,8 +30613,8 @@
       <c r="C38" s="1">
         <v>0</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>194</v>
+      <c r="D38" s="3" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30795,8 +30627,8 @@
       <c r="C39" s="1">
         <v>0</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>195</v>
+      <c r="D39" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30809,8 +30641,8 @@
       <c r="C40" s="1">
         <v>0</v>
       </c>
-      <c r="D40" s="4" t="s">
-        <v>207</v>
+      <c r="D40" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30823,8 +30655,8 @@
       <c r="C41" s="1">
         <v>0</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>196</v>
+      <c r="D41" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30837,8 +30669,8 @@
       <c r="C42" s="1">
         <v>0</v>
       </c>
-      <c r="D42" s="4" t="s">
-        <v>197</v>
+      <c r="D42" s="3" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30851,8 +30683,8 @@
       <c r="C43" s="1">
         <v>1</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>198</v>
+      <c r="D43" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30865,8 +30697,8 @@
       <c r="C44" s="1">
         <v>0</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>199</v>
+      <c r="D44" s="3" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30879,8 +30711,8 @@
       <c r="C45" s="1">
         <v>0</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>200</v>
+      <c r="D45" s="3" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30893,8 +30725,8 @@
       <c r="C46" s="1">
         <v>0</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>201</v>
+      <c r="D46" s="3" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30907,8 +30739,8 @@
       <c r="C47" s="1">
         <v>0</v>
       </c>
-      <c r="D47" s="4" t="s">
-        <v>202</v>
+      <c r="D47" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30921,8 +30753,8 @@
       <c r="C48" s="1">
         <v>0</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>203</v>
+      <c r="D48" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30935,8 +30767,8 @@
       <c r="C49" s="1">
         <v>1</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>204</v>
+      <c r="D49" s="3" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30949,8 +30781,8 @@
       <c r="C50" s="1">
         <v>0</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>205</v>
+      <c r="D50" s="3" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30963,8 +30795,8 @@
       <c r="C51" s="1">
         <v>0</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>206</v>
+      <c r="D51" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>